<commit_message>
updating blast furnace process (incomplete
</commit_message>
<xml_diff>
--- a/data/steel/SteelUnits_Relationships.xlsx
+++ b/data/steel/SteelUnits_Relationships.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Tanzer/GitHub/BlackBlox/data/steel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D899FD1E-1F3E-E64A-BDC5-981988C13299}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B02CFE2E-D8AA-4046-B257-4F087EF77D95}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="600" yWindow="1760" windowWidth="27120" windowHeight="15280" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="600" yWindow="1760" windowWidth="27120" windowHeight="15280" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Lime Kiln" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="425" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="407" uniqueCount="98">
   <si>
     <t>CaCO3</t>
   </si>
@@ -107,9 +107,6 @@
     <t>Hot Metal</t>
   </si>
   <si>
-    <t>Pulverized Coal</t>
-  </si>
-  <si>
     <t>Blast Furnace Gas Heat</t>
   </si>
   <si>
@@ -258,15 +255,6 @@
   </si>
   <si>
     <t>CO2 Capture Efficiency</t>
-  </si>
-  <si>
-    <t>Non-Coke Fuel</t>
-  </si>
-  <si>
-    <t>Biofuel</t>
-  </si>
-  <si>
-    <t>Biomass Cofiring Rate</t>
   </si>
   <si>
     <t>KnownQty</t>
@@ -731,7 +719,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
@@ -765,7 +753,7 @@
         <v>15</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
@@ -785,7 +773,7 @@
         <v>4</v>
       </c>
       <c r="F2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
@@ -805,7 +793,7 @@
         <v>4</v>
       </c>
       <c r="F3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
@@ -825,7 +813,7 @@
         <v>8</v>
       </c>
       <c r="F4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
@@ -836,24 +824,24 @@
         <v>3</v>
       </c>
       <c r="C5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E5" t="s">
         <v>8</v>
       </c>
       <c r="F5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B6" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C6" t="s">
         <v>17</v>
@@ -911,64 +899,64 @@
         <v>15</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>62</v>
+      </c>
+      <c r="B2" t="s">
         <v>63</v>
       </c>
-      <c r="B2" t="s">
-        <v>64</v>
-      </c>
       <c r="C2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
+        <v>62</v>
+      </c>
+      <c r="B3" t="s">
         <v>63</v>
-      </c>
-      <c r="B3" t="s">
-        <v>64</v>
       </c>
       <c r="C3" t="s">
         <v>5</v>
       </c>
       <c r="D3" t="s">
+        <v>64</v>
+      </c>
+      <c r="E3" t="s">
+        <v>8</v>
+      </c>
+      <c r="F3" t="s">
         <v>65</v>
-      </c>
-      <c r="E3" t="s">
-        <v>8</v>
-      </c>
-      <c r="F3" t="s">
-        <v>66</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
+        <v>62</v>
+      </c>
+      <c r="B4" t="s">
         <v>63</v>
-      </c>
-      <c r="B4" t="s">
-        <v>64</v>
       </c>
       <c r="C4" t="s">
         <v>9</v>
       </c>
       <c r="D4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E4" t="s">
         <v>8</v>
       </c>
       <c r="F4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
   </sheetData>
@@ -1022,16 +1010,16 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
+        <v>73</v>
+      </c>
+      <c r="D2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F2" t="s">
         <v>74</v>
-      </c>
-      <c r="D2" t="s">
-        <v>3</v>
-      </c>
-      <c r="E2" t="s">
-        <v>8</v>
-      </c>
-      <c r="F2" t="s">
-        <v>75</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
@@ -1045,13 +1033,13 @@
         <v>5</v>
       </c>
       <c r="D3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E3" t="s">
         <v>20</v>
       </c>
       <c r="F3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
@@ -1071,7 +1059,7 @@
         <v>8</v>
       </c>
       <c r="F4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
@@ -1082,7 +1070,7 @@
         <v>1</v>
       </c>
       <c r="C5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D5" t="s">
         <v>1</v>
@@ -1091,7 +1079,7 @@
         <v>8</v>
       </c>
       <c r="F5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
   </sheetData>
@@ -1137,7 +1125,7 @@
         <v>15</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
@@ -1157,7 +1145,7 @@
         <v>8</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
@@ -1168,27 +1156,27 @@
         <v>1</v>
       </c>
       <c r="C3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E3" t="s">
         <v>20</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B4" t="s">
         <v>1</v>
       </c>
       <c r="C4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D4" t="s">
         <v>3</v>
@@ -1197,7 +1185,7 @@
         <v>21</v>
       </c>
       <c r="F4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
@@ -1217,7 +1205,7 @@
         <v>8</v>
       </c>
       <c r="F5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
@@ -1228,7 +1216,7 @@
         <v>3</v>
       </c>
       <c r="C6" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D6" t="s">
         <v>1</v>
@@ -1237,7 +1225,7 @@
         <v>8</v>
       </c>
       <c r="F6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
   </sheetData>
@@ -1251,7 +1239,7 @@
   <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1284,7 +1272,7 @@
         <v>15</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
@@ -1298,13 +1286,13 @@
         <v>2</v>
       </c>
       <c r="D2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E2" t="s">
         <v>8</v>
       </c>
       <c r="F2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
@@ -1324,7 +1312,7 @@
         <v>20</v>
       </c>
       <c r="F3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
@@ -1344,7 +1332,7 @@
         <v>8</v>
       </c>
       <c r="F4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
@@ -1352,7 +1340,7 @@
         <v>2</v>
       </c>
       <c r="B5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C5" t="s">
         <v>0</v>
@@ -1364,7 +1352,7 @@
         <v>4</v>
       </c>
       <c r="F5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
@@ -1384,7 +1372,7 @@
         <v>4</v>
       </c>
       <c r="F6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
   </sheetData>
@@ -1430,7 +1418,7 @@
         <v>15</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
@@ -1438,7 +1426,7 @@
         <v>17</v>
       </c>
       <c r="B2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C2" t="s">
         <v>9</v>
@@ -1450,7 +1438,7 @@
         <v>21</v>
       </c>
       <c r="F2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
   </sheetData>
@@ -1496,7 +1484,7 @@
         <v>15</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
@@ -1516,7 +1504,7 @@
         <v>8</v>
       </c>
       <c r="F2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
@@ -1536,7 +1524,7 @@
         <v>20</v>
       </c>
       <c r="F3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
   </sheetData>
@@ -1546,10 +1534,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:I24"/>
+  <dimension ref="A1:I16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1564,31 +1552,31 @@
   <sheetData>
     <row r="1" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="E1" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="F1" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="G1" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="H1" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="E1" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>85</v>
-      </c>
-      <c r="H1" s="3" t="s">
-        <v>86</v>
-      </c>
       <c r="I1" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
@@ -1599,167 +1587,247 @@
         <v>3</v>
       </c>
       <c r="C2" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="D2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E2" t="s">
         <v>8</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="B3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C3" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="D3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E3" t="s">
         <v>8</v>
       </c>
       <c r="F3" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="B4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C4" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="D4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E4" t="s">
         <v>8</v>
       </c>
       <c r="F4" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
+        <v>83</v>
+      </c>
+      <c r="B5" t="s">
+        <v>66</v>
+      </c>
+      <c r="C5" t="s">
         <v>87</v>
       </c>
-      <c r="B5" t="s">
-        <v>67</v>
-      </c>
-      <c r="C5" t="s">
-        <v>91</v>
-      </c>
       <c r="D5" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E5" t="s">
         <v>8</v>
       </c>
       <c r="F5" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="B6" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C6" t="s">
+        <v>91</v>
+      </c>
+      <c r="D6" t="s">
         <v>95</v>
       </c>
-      <c r="D6" t="s">
-        <v>99</v>
-      </c>
       <c r="E6" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="F6" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="B7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C7" t="s">
+        <v>92</v>
+      </c>
+      <c r="D7" t="s">
+        <v>95</v>
+      </c>
+      <c r="E7" t="s">
         <v>96</v>
       </c>
-      <c r="D7" t="s">
-        <v>99</v>
-      </c>
-      <c r="E7" t="s">
-        <v>100</v>
-      </c>
       <c r="F7" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="B8" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C8" t="s">
+        <v>93</v>
+      </c>
+      <c r="D8" t="s">
+        <v>95</v>
+      </c>
+      <c r="E8" t="s">
+        <v>96</v>
+      </c>
+      <c r="F8" t="s">
         <v>97</v>
       </c>
-      <c r="D8" t="s">
-        <v>99</v>
-      </c>
-      <c r="E8" t="s">
-        <v>100</v>
-      </c>
-      <c r="F8" t="s">
-        <v>101</v>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>49</v>
+      </c>
+      <c r="B9" t="s">
+        <v>1</v>
+      </c>
+      <c r="C9" t="s">
+        <v>24</v>
+      </c>
+      <c r="D9" t="s">
+        <v>3</v>
+      </c>
+      <c r="E9" t="s">
+        <v>20</v>
+      </c>
+      <c r="F9" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>49</v>
+      </c>
+      <c r="B10" t="s">
+        <v>1</v>
+      </c>
+      <c r="C10" t="s">
+        <v>35</v>
+      </c>
+      <c r="D10" t="s">
+        <v>54</v>
+      </c>
+      <c r="E10" t="s">
+        <v>8</v>
+      </c>
+      <c r="F10" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>35</v>
+      </c>
+      <c r="B11" t="s">
+        <v>1</v>
+      </c>
+      <c r="C11" t="s">
+        <v>28</v>
+      </c>
+      <c r="D11" t="s">
+        <v>1</v>
+      </c>
+      <c r="E11" t="s">
+        <v>4</v>
+      </c>
+      <c r="F11" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
+        <v>35</v>
+      </c>
+      <c r="B12" t="s">
+        <v>1</v>
+      </c>
+      <c r="C12" t="s">
+        <v>5</v>
+      </c>
+      <c r="D12" t="s">
+        <v>3</v>
+      </c>
+      <c r="E12" t="s">
+        <v>4</v>
+      </c>
+      <c r="F12" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
         <v>24</v>
       </c>
-      <c r="B12" t="s">
-        <v>3</v>
-      </c>
-      <c r="C12" t="s">
+      <c r="B13" t="s">
+        <v>3</v>
+      </c>
+      <c r="C13" t="s">
         <v>16</v>
       </c>
-      <c r="D12" t="s">
-        <v>1</v>
-      </c>
-      <c r="E12" t="s">
-        <v>8</v>
-      </c>
-      <c r="F12" t="s">
-        <v>51</v>
+      <c r="D13" t="s">
+        <v>1</v>
+      </c>
+      <c r="E13" t="s">
+        <v>8</v>
+      </c>
+      <c r="F13" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>50</v>
+        <v>16</v>
       </c>
       <c r="B14" t="s">
         <v>1</v>
       </c>
       <c r="C14" t="s">
-        <v>24</v>
+        <v>38</v>
       </c>
       <c r="D14" t="s">
         <v>3</v>
@@ -1768,187 +1836,47 @@
         <v>20</v>
       </c>
       <c r="F14" t="s">
-        <v>60</v>
+        <v>39</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>50</v>
+        <v>16</v>
       </c>
       <c r="B15" t="s">
         <v>1</v>
       </c>
       <c r="C15" t="s">
-        <v>36</v>
+        <v>51</v>
       </c>
       <c r="D15" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E15" t="s">
         <v>8</v>
       </c>
       <c r="F15" t="s">
-        <v>60</v>
+        <v>39</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>36</v>
+        <v>51</v>
       </c>
       <c r="B16" t="s">
-        <v>1</v>
+        <v>54</v>
       </c>
       <c r="C16" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="D16" t="s">
-        <v>1</v>
+        <v>26</v>
       </c>
       <c r="E16" t="s">
-        <v>4</v>
+        <v>21</v>
       </c>
       <c r="F16" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
-        <v>36</v>
-      </c>
-      <c r="B17" t="s">
-        <v>1</v>
-      </c>
-      <c r="C17" t="s">
-        <v>5</v>
-      </c>
-      <c r="D17" t="s">
-        <v>3</v>
-      </c>
-      <c r="E17" t="s">
-        <v>4</v>
-      </c>
-      <c r="F17" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
-        <v>16</v>
-      </c>
-      <c r="B18" t="s">
-        <v>1</v>
-      </c>
-      <c r="C18" t="s">
-        <v>39</v>
-      </c>
-      <c r="D18" t="s">
-        <v>3</v>
-      </c>
-      <c r="E18" t="s">
-        <v>20</v>
-      </c>
-      <c r="F18" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
-        <v>16</v>
-      </c>
-      <c r="B19" t="s">
-        <v>1</v>
-      </c>
-      <c r="C19" t="s">
-        <v>52</v>
-      </c>
-      <c r="D19" t="s">
-        <v>55</v>
-      </c>
-      <c r="E19" t="s">
-        <v>8</v>
-      </c>
-      <c r="F19" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
-        <v>52</v>
-      </c>
-      <c r="B20" t="s">
-        <v>55</v>
-      </c>
-      <c r="C20" t="s">
-        <v>26</v>
-      </c>
-      <c r="D20" t="s">
-        <v>27</v>
-      </c>
-      <c r="E20" t="s">
-        <v>21</v>
-      </c>
-      <c r="F20" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
-        <v>76</v>
-      </c>
-      <c r="B22" t="s">
-        <v>55</v>
-      </c>
-      <c r="C22" t="s">
-        <v>77</v>
-      </c>
-      <c r="D22" t="s">
-        <v>1</v>
-      </c>
-      <c r="E22" t="s">
-        <v>8</v>
-      </c>
-      <c r="F22" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A23" t="s">
-        <v>77</v>
-      </c>
-      <c r="B23" t="s">
-        <v>1</v>
-      </c>
-      <c r="C23" t="s">
-        <v>26</v>
-      </c>
-      <c r="D23" t="s">
-        <v>27</v>
-      </c>
-      <c r="E23" t="s">
-        <v>21</v>
-      </c>
-      <c r="F23" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A24" t="s">
-        <v>76</v>
-      </c>
-      <c r="B24" t="s">
-        <v>55</v>
-      </c>
-      <c r="C24" t="s">
-        <v>25</v>
-      </c>
-      <c r="D24" t="s">
-        <v>1</v>
-      </c>
-      <c r="E24" t="s">
-        <v>20</v>
-      </c>
-      <c r="F24" t="s">
-        <v>78</v>
+        <v>47</v>
       </c>
     </row>
   </sheetData>
@@ -1994,38 +1922,38 @@
         <v>15</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B2" t="s">
         <v>3</v>
       </c>
       <c r="C2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E2" t="s">
         <v>20</v>
       </c>
       <c r="F2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B3" t="s">
         <v>3</v>
       </c>
       <c r="C3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D3" t="s">
         <v>1</v>
@@ -2034,7 +1962,7 @@
         <v>8</v>
       </c>
       <c r="F3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
@@ -2045,16 +1973,16 @@
         <v>1</v>
       </c>
       <c r="C4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E4" t="s">
         <v>20</v>
       </c>
       <c r="F4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
@@ -2065,47 +1993,47 @@
         <v>1</v>
       </c>
       <c r="C5" t="s">
+        <v>35</v>
+      </c>
+      <c r="D5" t="s">
+        <v>55</v>
+      </c>
+      <c r="E5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F5" t="s">
         <v>36</v>
-      </c>
-      <c r="D5" t="s">
-        <v>56</v>
-      </c>
-      <c r="E5" t="s">
-        <v>8</v>
-      </c>
-      <c r="F5" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B6" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C6" t="s">
         <v>5</v>
       </c>
       <c r="D6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E6" t="s">
         <v>4</v>
       </c>
       <c r="F6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D7" t="s">
         <v>1</v>
@@ -2114,7 +2042,7 @@
         <v>4</v>
       </c>
       <c r="F7" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
@@ -2134,7 +2062,7 @@
         <v>8</v>
       </c>
       <c r="F8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
@@ -2154,7 +2082,7 @@
         <v>8</v>
       </c>
       <c r="F9" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
   </sheetData>
@@ -2200,32 +2128,32 @@
         <v>15</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B2" t="s">
         <v>1</v>
       </c>
       <c r="C2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" t="s">
+        <v>61</v>
+      </c>
+      <c r="F2" t="s">
         <v>33</v>
-      </c>
-      <c r="D2" t="s">
-        <v>3</v>
-      </c>
-      <c r="E2" t="s">
-        <v>62</v>
-      </c>
-      <c r="F2" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B3" t="s">
         <v>3</v>
@@ -2240,7 +2168,7 @@
         <v>8</v>
       </c>
       <c r="F3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
   </sheetData>
@@ -2286,12 +2214,12 @@
         <v>15</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B2" t="s">
         <v>3</v>
@@ -2306,38 +2234,38 @@
         <v>8</v>
       </c>
       <c r="F2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B3" t="s">
         <v>1</v>
       </c>
       <c r="C3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E3" t="s">
         <v>8</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B4" t="s">
         <v>1</v>
       </c>
       <c r="C4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D4" t="s">
         <v>3</v>
@@ -2346,38 +2274,38 @@
         <v>20</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B5" t="s">
+        <v>66</v>
+      </c>
+      <c r="C5" t="s">
+        <v>28</v>
+      </c>
+      <c r="D5" t="s">
         <v>67</v>
       </c>
-      <c r="C5" t="s">
-        <v>29</v>
-      </c>
-      <c r="D5" t="s">
+      <c r="E5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F5" t="s">
         <v>68</v>
-      </c>
-      <c r="E5" t="s">
-        <v>8</v>
-      </c>
-      <c r="F5" t="s">
-        <v>69</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
+        <v>69</v>
+      </c>
+      <c r="B6" t="s">
+        <v>66</v>
+      </c>
+      <c r="C6" t="s">
         <v>70</v>
-      </c>
-      <c r="B6" t="s">
-        <v>67</v>
-      </c>
-      <c r="C6" t="s">
-        <v>71</v>
       </c>
       <c r="D6" t="s">
         <v>3</v>
@@ -2386,7 +2314,7 @@
         <v>20</v>
       </c>
       <c r="F6" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added minor comment to SteelUnits_Relationships.xlsx
</commit_message>
<xml_diff>
--- a/data/steel/SteelUnits_Relationships.xlsx
+++ b/data/steel/SteelUnits_Relationships.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10304"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\setanzer\GitHub\BlackBlox\data\steel\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="1" documentId="11_2581BD2C224B2290F0C32EA0A6558C7801965D61" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{5860405D-EE2F-0E4B-AF23-A72FBD6DC315}"/>
   <bookViews>
-    <workbookView xWindow="600" yWindow="2355" windowWidth="27120" windowHeight="15285" firstSheet="1" activeTab="1"/>
+    <workbookView xWindow="600" yWindow="2355" windowWidth="27120" windowHeight="15285" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Lime Kiln" sheetId="1" r:id="rId1"/>
@@ -24,12 +25,19 @@
     <sheet name="Electric Arc Furnace" sheetId="11" r:id="rId10"/>
     <sheet name="CO2 Capture" sheetId="12" r:id="rId11"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191028"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="472" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="472" uniqueCount="121">
   <si>
     <t>CaCO3</t>
   </si>
@@ -358,9 +366,6 @@
     <t>energy in coking coal (LHV)</t>
   </si>
   <si>
-    <t>coke oven gas heat</t>
-  </si>
-  <si>
     <t>combustion-lhv-noenergyin</t>
   </si>
   <si>
@@ -389,12 +394,15 @@
   </si>
   <si>
     <t>consumed heat and electricity</t>
+  </si>
+  <si>
+    <t>coke oven gas heat (LHV)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -537,6 +545,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -572,6 +597,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -747,24 +789,24 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView workbookViewId="0" xr3:uid="{AEA406A1-0E4B-5B11-9CD5-51D6E497D94C}">
       <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.296875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.43359375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="24.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.6796875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.73828125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="24.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>9</v>
       </c>
@@ -787,7 +829,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -807,7 +849,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -827,7 +869,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -847,7 +889,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>2</v>
       </c>
@@ -867,7 +909,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>41</v>
       </c>
@@ -893,24 +935,24 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:G4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView workbookViewId="0" xr3:uid="{7BE570AB-09E9-518F-B8F7-3F91B7162CA9}">
       <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.296875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.43359375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="24.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.6796875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.73828125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="24.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>9</v>
       </c>
@@ -933,7 +975,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>58</v>
       </c>
@@ -950,7 +992,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>58</v>
       </c>
@@ -970,7 +1012,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>58</v>
       </c>
@@ -996,24 +1038,24 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1:F5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView workbookViewId="0" xr3:uid="{65FA3815-DCC1-5481-872F-D2879ED395ED}">
       <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.296875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.43359375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="24.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.6796875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.73828125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="24.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>9</v>
       </c>
@@ -1033,7 +1075,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -1053,7 +1095,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -1073,7 +1115,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -1093,7 +1135,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -1119,25 +1161,25 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:I18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C30" sqref="C30"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0" xr3:uid="{958C4451-9541-5A59-BF78-D2F731DF1C81}">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="36.42578125" customWidth="1"/>
-    <col min="2" max="2" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="25.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="22.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="24.85546875" customWidth="1"/>
+    <col min="1" max="1" width="36.453125" customWidth="1"/>
+    <col min="2" max="2" width="11.43359375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="25.15234375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.22265625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.73828125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="22.328125" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="24.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>71</v>
       </c>
@@ -1166,7 +1208,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="2" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>87</v>
       </c>
@@ -1174,7 +1216,7 @@
         <v>63</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>63</v>
@@ -1186,9 +1228,9 @@
         <v>101</v>
       </c>
     </row>
-    <row r="3" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>102</v>
@@ -1206,15 +1248,15 @@
         <v>100</v>
       </c>
     </row>
-    <row r="4" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>102</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>102</v>
@@ -1223,9 +1265,9 @@
         <v>104</v>
       </c>
     </row>
-    <row r="5" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>102</v>
@@ -1246,9 +1288,9 @@
       <c r="H5" s="2"/>
       <c r="I5" s="2"/>
     </row>
-    <row r="6" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>102</v>
@@ -1269,7 +1311,7 @@
       <c r="H6" s="2"/>
       <c r="I6" s="2"/>
     </row>
-    <row r="7" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>107</v>
       </c>
@@ -1292,7 +1334,7 @@
       <c r="H7" s="2"/>
       <c r="I7" s="2"/>
     </row>
-    <row r="8" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>108</v>
       </c>
@@ -1315,7 +1357,7 @@
       <c r="H8" s="2"/>
       <c r="I8" s="2"/>
     </row>
-    <row r="9" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
         <v>93</v>
       </c>
@@ -1323,7 +1365,7 @@
         <v>98</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>102</v>
@@ -1338,7 +1380,7 @@
       <c r="H9" s="2"/>
       <c r="I9" s="2"/>
     </row>
-    <row r="10" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
         <v>97</v>
       </c>
@@ -1346,7 +1388,7 @@
         <v>98</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D10" s="2" t="s">
         <v>102</v>
@@ -1361,9 +1403,9 @@
       <c r="H10" s="2"/>
       <c r="I10" s="2"/>
     </row>
-    <row r="11" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>102</v>
@@ -1375,18 +1417,18 @@
         <v>102</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="G11" s="2"/>
       <c r="H11" s="2"/>
       <c r="I11" s="2"/>
     </row>
-    <row r="12" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>102</v>
@@ -1398,16 +1440,16 @@
         <v>102</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="G12" s="2"/>
       <c r="H12" s="2"/>
       <c r="I12" s="2"/>
     </row>
-    <row r="13" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
         <v>105</v>
       </c>
@@ -1415,7 +1457,7 @@
         <v>102</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>109</v>
+        <v>119</v>
       </c>
       <c r="D13" s="2" t="s">
         <v>63</v>
@@ -1433,7 +1475,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
         <v>87</v>
       </c>
@@ -1441,7 +1483,7 @@
         <v>3</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D14" s="2" t="s">
         <v>1</v>
@@ -1456,7 +1498,7 @@
       <c r="H14" s="2"/>
       <c r="I14" s="2"/>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
         <v>87</v>
       </c>
@@ -1464,7 +1506,7 @@
         <v>3</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D15" s="2" t="s">
         <v>1</v>
@@ -1479,15 +1521,15 @@
       <c r="H15" s="2"/>
       <c r="I15" s="2"/>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B16" s="2" t="s">
         <v>98</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D16" s="2" t="s">
         <v>63</v>
@@ -1499,14 +1541,14 @@
         <v>101</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="H16" s="2" t="s">
         <v>98</v>
       </c>
       <c r="I16" s="2"/>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A17" s="2"/>
       <c r="B17" s="2"/>
       <c r="C17" s="2"/>
@@ -1517,7 +1559,7 @@
       <c r="H17" s="2"/>
       <c r="I17" s="2"/>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18" s="2"/>
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>
@@ -1535,24 +1577,24 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:G6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView workbookViewId="0" xr3:uid="{842E5F09-E766-5B8D-85AF-A39847EA96FD}">
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.296875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.43359375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="24.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.6796875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.73828125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="24.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>9</v>
       </c>
@@ -1575,7 +1617,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>15</v>
       </c>
@@ -1595,7 +1637,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>15</v>
       </c>
@@ -1615,7 +1657,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>15</v>
       </c>
@@ -1635,7 +1677,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>2</v>
       </c>
@@ -1655,7 +1697,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>0</v>
       </c>
@@ -1681,24 +1723,24 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView workbookViewId="0" xr3:uid="{51F8DEE0-4D01-5F28-A812-FC0BD7CAC4A5}">
       <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.296875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.43359375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="24.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.6796875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.73828125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="24.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>9</v>
       </c>
@@ -1721,7 +1763,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>16</v>
       </c>
@@ -1747,24 +1789,24 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:G3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView workbookViewId="0" xr3:uid="{F9CF3CF3-643B-5BE6-8B46-32C596A47465}">
       <selection activeCell="D36" sqref="D36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="17" customWidth="1"/>
-    <col min="2" max="2" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="24.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.94921875" customWidth="1"/>
+    <col min="2" max="2" width="11.43359375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.19921875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.6796875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.73828125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="24.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>9</v>
       </c>
@@ -1787,7 +1829,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>17</v>
       </c>
@@ -1807,7 +1849,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>17</v>
       </c>
@@ -1833,24 +1875,24 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:I16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView workbookViewId="0" xr3:uid="{78B4E459-6924-5F8B-B7BA-2DD04133E49E}">
       <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="21.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="24.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.296875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.43359375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.1171875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.6796875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.73828125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="24.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>71</v>
       </c>
@@ -1879,7 +1921,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>23</v>
       </c>
@@ -1899,7 +1941,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>79</v>
       </c>
@@ -1919,7 +1961,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>79</v>
       </c>
@@ -1939,7 +1981,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>79</v>
       </c>
@@ -1959,7 +2001,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>81</v>
       </c>
@@ -1979,7 +2021,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>89</v>
       </c>
@@ -1999,7 +2041,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>83</v>
       </c>
@@ -2019,7 +2061,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>46</v>
       </c>
@@ -2039,7 +2081,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>46</v>
       </c>
@@ -2059,7 +2101,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>34</v>
       </c>
@@ -2079,7 +2121,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>34</v>
       </c>
@@ -2099,7 +2141,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>23</v>
       </c>
@@ -2119,7 +2161,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>15</v>
       </c>
@@ -2139,7 +2181,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>15</v>
       </c>
@@ -2159,7 +2201,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>48</v>
       </c>
@@ -2185,24 +2227,24 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:G9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView workbookViewId="0" xr3:uid="{9B253EF2-77E0-53E3-AE26-4D66ECD923F3}">
       <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.296875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.43359375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="24.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.6796875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.73828125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="24.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>9</v>
       </c>
@@ -2225,7 +2267,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>26</v>
       </c>
@@ -2245,7 +2287,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>26</v>
       </c>
@@ -2265,7 +2307,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>23</v>
       </c>
@@ -2285,7 +2327,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>23</v>
       </c>
@@ -2305,7 +2347,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>34</v>
       </c>
@@ -2325,7 +2367,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>34</v>
       </c>
@@ -2345,7 +2387,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>23</v>
       </c>
@@ -2365,7 +2407,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>23</v>
       </c>
@@ -2391,24 +2433,24 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:G3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView workbookViewId="0" xr3:uid="{85D5C41F-068E-5C55-9968-509E7C2A5619}">
       <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.296875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.43359375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="24.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.6796875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.73828125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="24.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>9</v>
       </c>
@@ -2431,7 +2473,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>26</v>
       </c>
@@ -2451,7 +2493,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>31</v>
       </c>
@@ -2477,24 +2519,24 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:G6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView workbookViewId="0" xr3:uid="{44B22561-5205-5C8A-B808-2C70100D228F}">
       <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.296875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.43359375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="24.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.6796875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.73828125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="24.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>9</v>
       </c>
@@ -2517,7 +2559,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>27</v>
       </c>
@@ -2537,7 +2579,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>30</v>
       </c>
@@ -2557,7 +2599,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>30</v>
       </c>
@@ -2577,7 +2619,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>65</v>
       </c>
@@ -2597,7 +2639,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>65</v>
       </c>

</xml_diff>

<commit_message>
process calculations from IEAGHG 2013 reference steel mill
</commit_message>
<xml_diff>
--- a/data/steel/SteelUnits_Relationships.xlsx
+++ b/data/steel/SteelUnits_Relationships.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10304"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\setanzer\GitHub\BlackBlox\data\steel\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="159" documentId="11_A19A31F9276096631CB14E3BEEA1936904EB5EDF" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{F572C694-20A8-B649-ADF0-38621821A61D}"/>
   <bookViews>
-    <workbookView xWindow="600" yWindow="2355" windowWidth="27120" windowHeight="15285" activeTab="3"/>
+    <workbookView xWindow="600" yWindow="2355" windowWidth="27120" windowHeight="15285" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Lime Kiln" sheetId="1" r:id="rId1"/>
@@ -19,12 +20,13 @@
     <sheet name="Power Plant" sheetId="4" r:id="rId5"/>
     <sheet name="Heat Recovery" sheetId="9" r:id="rId6"/>
     <sheet name="BOF Steelmaking" sheetId="6" r:id="rId7"/>
-    <sheet name="Rolling" sheetId="7" r:id="rId8"/>
-    <sheet name="Air Seperation" sheetId="8" r:id="rId9"/>
-    <sheet name="Electric Arc Furnace" sheetId="11" r:id="rId10"/>
-    <sheet name="CO2 Capture" sheetId="12" r:id="rId11"/>
+    <sheet name="Ladle Metallurgy" sheetId="13" r:id="rId8"/>
+    <sheet name="Forming" sheetId="7" r:id="rId9"/>
+    <sheet name="Air Seperation" sheetId="8" r:id="rId10"/>
+    <sheet name="Electric Arc Furnace" sheetId="11" r:id="rId11"/>
+    <sheet name="CO2 Capture" sheetId="12" r:id="rId12"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -36,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="761" uniqueCount="172">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="896" uniqueCount="204">
   <si>
     <t>CaCO3</t>
   </si>
@@ -86,18 +88,12 @@
     <t>Waste Heat</t>
   </si>
   <si>
-    <t>Steam Heat</t>
-  </si>
-  <si>
     <t>Remainder</t>
   </si>
   <si>
     <t>Combustion</t>
   </si>
   <si>
-    <t>Combustion Efficiency</t>
-  </si>
-  <si>
     <t>Recovered Heat</t>
   </si>
   <si>
@@ -125,15 +121,9 @@
     <t>Rolled Steel</t>
   </si>
   <si>
-    <t>Rolled-to-Liquid Ratio</t>
-  </si>
-  <si>
     <t>Electricity Demand</t>
   </si>
   <si>
-    <t>C</t>
-  </si>
-  <si>
     <t>Carbon Content of Hot Metal</t>
   </si>
   <si>
@@ -161,15 +151,9 @@
     <t>Sinter Demand</t>
   </si>
   <si>
-    <t>Iron</t>
-  </si>
-  <si>
     <t>Steel Scrap</t>
   </si>
   <si>
-    <t>Temporary</t>
-  </si>
-  <si>
     <t xml:space="preserve">Temporary </t>
   </si>
   <si>
@@ -552,12 +536,120 @@
   </si>
   <si>
     <t>sinter Fe in hot metal</t>
+  </si>
+  <si>
+    <t>Hot metal</t>
+  </si>
+  <si>
+    <t>Metal inflow</t>
+  </si>
+  <si>
+    <t>Metal Demand</t>
+  </si>
+  <si>
+    <t>C__in hot metal</t>
+  </si>
+  <si>
+    <t>Flux</t>
+  </si>
+  <si>
+    <t>Flux demand</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Metal outflows </t>
+  </si>
+  <si>
+    <t>Slag</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Subtraction </t>
+  </si>
+  <si>
+    <t>Total Flux</t>
+  </si>
+  <si>
+    <t>Lime in Flux</t>
+  </si>
+  <si>
+    <t>Ladled Steel</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Electricity </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Inflow </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ratio </t>
+  </si>
+  <si>
+    <t>Electricity demand</t>
+  </si>
+  <si>
+    <t>Heat demand</t>
+  </si>
+  <si>
+    <t>Steel scrap</t>
+  </si>
+  <si>
+    <t>Scrap Demand</t>
+  </si>
+  <si>
+    <t>Alloying metals</t>
+  </si>
+  <si>
+    <t>Alloy demand</t>
+  </si>
+  <si>
+    <t>Scrap demand</t>
+  </si>
+  <si>
+    <t>Other metals</t>
+  </si>
+  <si>
+    <t>Temp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Addition </t>
+  </si>
+  <si>
+    <t>Subtraction</t>
+  </si>
+  <si>
+    <t>Oxygen demand</t>
+  </si>
+  <si>
+    <t>Total flux</t>
+  </si>
+  <si>
+    <t>Flux Demand</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Total flux </t>
+  </si>
+  <si>
+    <t>CaO fraction of flux</t>
+  </si>
+  <si>
+    <t>Oxygen</t>
+  </si>
+  <si>
+    <t>Forming Losses</t>
+  </si>
+  <si>
+    <t>Scrap</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Oxygen </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Oxygen demand </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -582,12 +674,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -602,11 +700,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -700,6 +800,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -735,6 +852,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -910,24 +1044,24 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:G5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:E3"/>
+    <sheetView workbookViewId="0" xr3:uid="{AEA406A1-0E4B-5B11-9CD5-51D6E497D94C}">
+      <selection activeCell="A6" sqref="A6:XFD6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.296875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.43359375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="24.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.6796875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.73828125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="24.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>8</v>
       </c>
@@ -947,10 +1081,10 @@
         <v>13</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -967,10 +1101,10 @@
         <v>4</v>
       </c>
       <c r="F2" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -987,10 +1121,10 @@
         <v>4</v>
       </c>
       <c r="F3" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -1007,10 +1141,10 @@
         <v>6</v>
       </c>
       <c r="F4" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>2</v>
       </c>
@@ -1018,36 +1152,16 @@
         <v>3</v>
       </c>
       <c r="C5" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="D5" t="s">
-        <v>43</v>
+        <v>1</v>
       </c>
       <c r="E5" t="s">
         <v>6</v>
       </c>
       <c r="F5" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>35</v>
-      </c>
-      <c r="B6" t="s">
-        <v>43</v>
-      </c>
-      <c r="C6" t="s">
-        <v>14</v>
-      </c>
-      <c r="D6" t="s">
-        <v>1</v>
-      </c>
-      <c r="E6" t="s">
-        <v>18</v>
-      </c>
-      <c r="F6" t="s">
-        <v>19</v>
+        <v>31</v>
       </c>
     </row>
   </sheetData>
@@ -1056,24 +1170,24 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
+  <dimension ref="A1:G7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G1" sqref="G1"/>
+    <sheetView topLeftCell="D4" workbookViewId="0" xr3:uid="{44B22561-5205-5C8A-B808-2C70100D228F}">
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.296875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.43359375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="24.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.6796875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.73828125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="24.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>8</v>
       </c>
@@ -1093,64 +1207,127 @@
         <v>13</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>49</v>
+        <v>22</v>
       </c>
       <c r="B2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" t="s">
         <v>50</v>
       </c>
-      <c r="C2" t="s">
-        <v>42</v>
-      </c>
-      <c r="D2" t="s">
-        <v>37</v>
-      </c>
-      <c r="E2" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>49</v>
-      </c>
-      <c r="B3" t="s">
-        <v>50</v>
-      </c>
-      <c r="C3" t="s">
-        <v>5</v>
-      </c>
       <c r="D3" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="E3" t="s">
         <v>6</v>
       </c>
-      <c r="F3" t="s">
+      <c r="F3" s="2" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" t="s">
+        <v>24</v>
+      </c>
+      <c r="D4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E4" t="s">
+        <v>16</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>50</v>
+      </c>
+      <c r="B5" t="s">
+        <v>47</v>
+      </c>
+      <c r="C5" t="s">
+        <v>22</v>
+      </c>
+      <c r="D5" t="s">
+        <v>48</v>
+      </c>
+      <c r="E5" t="s">
+        <v>6</v>
+      </c>
+      <c r="F5" t="s">
         <v>49</v>
       </c>
-      <c r="B4" t="s">
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
         <v>50</v>
       </c>
-      <c r="C4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D4" t="s">
-        <v>37</v>
-      </c>
-      <c r="E4" t="s">
+      <c r="B6" t="s">
+        <v>47</v>
+      </c>
+      <c r="C6" t="s">
+        <v>51</v>
+      </c>
+      <c r="D6" t="s">
+        <v>3</v>
+      </c>
+      <c r="E6" t="s">
+        <v>16</v>
+      </c>
+      <c r="F6" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>22</v>
+      </c>
+      <c r="B7" t="s">
+        <v>3</v>
+      </c>
+      <c r="C7" t="s">
+        <v>32</v>
+      </c>
+      <c r="D7" t="s">
+        <v>1</v>
+      </c>
+      <c r="E7" t="s">
         <v>6</v>
       </c>
-      <c r="F4" t="s">
-        <v>30</v>
+      <c r="F7" t="s">
+        <v>182</v>
       </c>
     </row>
   </sheetData>
@@ -1159,24 +1336,127 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
+  <dimension ref="A1:G4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0" xr3:uid="{7BE570AB-09E9-518F-B8F7-3F91B7162CA9}">
+      <selection activeCell="G1" sqref="G1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="11.296875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.43359375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.6796875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.73828125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="24.88671875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B2" t="s">
+        <v>44</v>
+      </c>
+      <c r="C2" t="s">
+        <v>37</v>
+      </c>
+      <c r="D2" t="s">
+        <v>33</v>
+      </c>
+      <c r="E2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>43</v>
+      </c>
+      <c r="B3" t="s">
+        <v>44</v>
+      </c>
+      <c r="C3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" t="s">
+        <v>45</v>
+      </c>
+      <c r="E3" t="s">
+        <v>6</v>
+      </c>
+      <c r="F3" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>43</v>
+      </c>
+      <c r="B4" t="s">
+        <v>44</v>
+      </c>
+      <c r="C4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" t="s">
+        <v>33</v>
+      </c>
+      <c r="E4" t="s">
+        <v>6</v>
+      </c>
+      <c r="F4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1:F5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView workbookViewId="0" xr3:uid="{65FA3815-DCC1-5481-872F-D2879ED395ED}">
       <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.296875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.43359375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="24.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.6796875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.73828125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="24.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>8</v>
       </c>
@@ -1196,7 +1476,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -1204,7 +1484,7 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="D2" t="s">
         <v>3</v>
@@ -1213,10 +1493,10 @@
         <v>6</v>
       </c>
       <c r="F2" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -1227,16 +1507,16 @@
         <v>5</v>
       </c>
       <c r="D3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F3" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -1253,10 +1533,10 @@
         <v>6</v>
       </c>
       <c r="F4" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -1264,7 +1544,7 @@
         <v>1</v>
       </c>
       <c r="C5" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="D5" t="s">
         <v>1</v>
@@ -1273,7 +1553,7 @@
         <v>6</v>
       </c>
       <c r="F5" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
     </row>
   </sheetData>
@@ -1282,329 +1562,329 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:I18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView workbookViewId="0" xr3:uid="{958C4451-9541-5A59-BF78-D2F731DF1C81}">
       <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="36.42578125" customWidth="1"/>
-    <col min="2" max="2" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="25.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="22.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="24.85546875" customWidth="1"/>
+    <col min="1" max="1" width="36.453125" customWidth="1"/>
+    <col min="2" max="2" width="11.43359375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="25.15234375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.22265625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.73828125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="22.328125" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="24.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="E1" s="1" t="s">
+      <c r="I1" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="H1" s="1" t="s">
+      <c r="B2" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="E3" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="I1" s="1" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+      <c r="F3" s="2" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="D5" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>78</v>
-      </c>
       <c r="E5" s="2" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="G5" s="2"/>
       <c r="H5" s="2"/>
       <c r="I5" s="2"/>
     </row>
-    <row r="6" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="B6" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="C6" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="C6" s="2" t="s">
-        <v>88</v>
-      </c>
       <c r="D6" s="2" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="G6" s="2"/>
       <c r="H6" s="2"/>
       <c r="I6" s="2"/>
     </row>
-    <row r="7" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="B7" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="E7" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="C7" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>84</v>
-      </c>
       <c r="F7" s="2" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="G7" s="2"/>
       <c r="H7" s="2"/>
       <c r="I7" s="2"/>
     </row>
-    <row r="8" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="B8" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="E8" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="C8" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>84</v>
-      </c>
       <c r="F8" s="2" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="G8" s="2"/>
       <c r="H8" s="2"/>
       <c r="I8" s="2"/>
     </row>
-    <row r="9" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="F9" s="2" t="s">
         <v>74</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="E9" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="F9" s="2" t="s">
-        <v>80</v>
       </c>
       <c r="G9" s="2"/>
       <c r="H9" s="2"/>
       <c r="I9" s="2"/>
     </row>
-    <row r="10" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="G10" s="2"/>
       <c r="H10" s="2"/>
       <c r="I10" s="2"/>
     </row>
-    <row r="11" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="C11" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="F11" s="2" t="s">
         <v>85</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="E11" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="F11" s="2" t="s">
-        <v>91</v>
       </c>
       <c r="G11" s="2"/>
       <c r="H11" s="2"/>
       <c r="I11" s="2"/>
     </row>
-    <row r="12" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="G12" s="2"/>
       <c r="H12" s="2"/>
       <c r="I12" s="2"/>
     </row>
-    <row r="13" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="H13" s="2" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="B14" s="2" t="s">
         <v>3</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="D14" s="2" t="s">
         <v>1</v>
@@ -1613,21 +1893,21 @@
         <v>6</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="G14" s="2"/>
       <c r="H14" s="2"/>
       <c r="I14" s="2"/>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>3</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="D15" s="2" t="s">
         <v>1</v>
@@ -1636,40 +1916,40 @@
         <v>6</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="G15" s="2"/>
       <c r="H15" s="2"/>
       <c r="I15" s="2"/>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="H16" s="2" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="I16" s="2"/>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A17" s="2"/>
       <c r="B17" s="2"/>
       <c r="C17" s="2"/>
@@ -1680,7 +1960,7 @@
       <c r="H17" s="2"/>
       <c r="I17" s="2"/>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18" s="2"/>
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>
@@ -1698,56 +1978,56 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:I25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView workbookViewId="0" xr3:uid="{842E5F09-E766-5B8D-85AF-A39847EA96FD}">
       <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="21.140625" customWidth="1"/>
-    <col min="2" max="2" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.1171875" customWidth="1"/>
+    <col min="2" max="2" width="11.43359375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="24.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.28515625" customWidth="1"/>
+    <col min="4" max="4" width="16.6796875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.73828125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="24.88671875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>69</v>
-      </c>
       <c r="I1" s="1" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="B2" t="s">
         <v>3</v>
@@ -1762,247 +2042,247 @@
         <v>6</v>
       </c>
       <c r="F2" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="B3" t="s">
         <v>3</v>
       </c>
       <c r="C3" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="D3" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="E3" t="s">
         <v>6</v>
       </c>
       <c r="F3" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="B4" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="C4" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="D4" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="E4" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
       <c r="B5" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="C5" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="D5" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="E5" t="s">
         <v>6</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="B6" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="C6" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="D6" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="E6" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="B7" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="C7" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
       <c r="D7" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="E7" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
       <c r="B8" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="C8" t="s">
-        <v>150</v>
+        <v>144</v>
       </c>
       <c r="D8" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="E8" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>150</v>
+        <v>144</v>
       </c>
       <c r="B9" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="C9" t="s">
         <v>5</v>
       </c>
       <c r="D9" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="E9" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="B10" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="C10" t="s">
+        <v>109</v>
+      </c>
+      <c r="D10" t="s">
+        <v>76</v>
+      </c>
+      <c r="E10" t="s">
+        <v>77</v>
+      </c>
+      <c r="G10" t="s">
         <v>115</v>
       </c>
-      <c r="D10" t="s">
-        <v>82</v>
-      </c>
-      <c r="E10" t="s">
-        <v>83</v>
-      </c>
-      <c r="G10" t="s">
-        <v>121</v>
-      </c>
       <c r="H10" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>150</v>
+        <v>144</v>
       </c>
       <c r="B11" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="C11" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="D11" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="E11" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="I11" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
       <c r="B12" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="C12" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="D12" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="E12" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
       <c r="G12" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="H12" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="B13" t="s">
         <v>3</v>
       </c>
       <c r="C13" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="D13" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="E13" t="s">
         <v>6</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="B14" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="C14" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="D14" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="E14" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
       <c r="F14" s="2"/>
       <c r="G14" s="2" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="H14" s="2" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="B15" t="s">
         <v>3</v>
@@ -2017,18 +2297,18 @@
         <v>6</v>
       </c>
       <c r="F15" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="B16" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="C16" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="D16" t="s">
         <v>1</v>
@@ -2037,193 +2317,193 @@
         <v>6</v>
       </c>
       <c r="F16" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="B17" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="C17" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="D17" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="E17" t="s">
         <v>6</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="B18" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="C18" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="D18" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="E18" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="F18" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="B19" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="C19" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="D19" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="E19" t="s">
         <v>6</v>
       </c>
       <c r="F19" s="2" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>96</v>
+      </c>
+      <c r="B20" t="s">
+        <v>76</v>
+      </c>
+      <c r="C20" t="s">
+        <v>106</v>
+      </c>
+      <c r="D20" t="s">
+        <v>72</v>
+      </c>
+      <c r="E20" t="s">
+        <v>16</v>
+      </c>
+      <c r="F20" s="2" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>98</v>
+      </c>
+      <c r="B21" t="s">
+        <v>72</v>
+      </c>
+      <c r="C21" t="s">
+        <v>68</v>
+      </c>
+      <c r="D21" t="s">
+        <v>72</v>
+      </c>
+      <c r="E21" t="s">
+        <v>97</v>
+      </c>
+      <c r="F21" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>106</v>
+      </c>
+      <c r="B22" t="s">
+        <v>72</v>
+      </c>
+      <c r="C22" t="s">
+        <v>66</v>
+      </c>
+      <c r="D22" t="s">
+        <v>72</v>
+      </c>
+      <c r="E22" t="s">
+        <v>97</v>
+      </c>
+      <c r="F22" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>68</v>
+      </c>
+      <c r="B23" t="s">
+        <v>72</v>
+      </c>
+      <c r="C23" t="s">
+        <v>103</v>
+      </c>
+      <c r="D23" t="s">
+        <v>76</v>
+      </c>
+      <c r="E23" t="s">
+        <v>67</v>
+      </c>
+      <c r="F23" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>66</v>
+      </c>
+      <c r="B24" t="s">
+        <v>72</v>
+      </c>
+      <c r="C24" t="s">
+        <v>104</v>
+      </c>
+      <c r="D24" t="s">
+        <v>76</v>
+      </c>
+      <c r="E24" t="s">
+        <v>67</v>
+      </c>
+      <c r="F24" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>104</v>
+      </c>
+      <c r="B25" t="s">
+        <v>76</v>
+      </c>
+      <c r="C25" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>102</v>
-      </c>
-      <c r="B20" t="s">
-        <v>82</v>
-      </c>
-      <c r="C20" t="s">
-        <v>112</v>
-      </c>
-      <c r="D20" t="s">
-        <v>78</v>
-      </c>
-      <c r="E20" t="s">
-        <v>17</v>
-      </c>
-      <c r="F20" s="2" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
+      <c r="D25" t="s">
+        <v>48</v>
+      </c>
+      <c r="E25" t="s">
+        <v>77</v>
+      </c>
+      <c r="F25" t="s">
+        <v>75</v>
+      </c>
+      <c r="G25" t="s">
         <v>104</v>
       </c>
-      <c r="B21" t="s">
-        <v>78</v>
-      </c>
-      <c r="C21" t="s">
-        <v>74</v>
-      </c>
-      <c r="D21" t="s">
-        <v>78</v>
-      </c>
-      <c r="E21" t="s">
-        <v>103</v>
-      </c>
-      <c r="F21" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>112</v>
-      </c>
-      <c r="B22" t="s">
-        <v>78</v>
-      </c>
-      <c r="C22" t="s">
-        <v>72</v>
-      </c>
-      <c r="D22" t="s">
-        <v>78</v>
-      </c>
-      <c r="E22" t="s">
-        <v>103</v>
-      </c>
-      <c r="F22" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>74</v>
-      </c>
-      <c r="B23" t="s">
-        <v>78</v>
-      </c>
-      <c r="C23" t="s">
-        <v>109</v>
-      </c>
-      <c r="D23" t="s">
-        <v>82</v>
-      </c>
-      <c r="E23" t="s">
-        <v>73</v>
-      </c>
-      <c r="F23" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>72</v>
-      </c>
-      <c r="B24" t="s">
-        <v>78</v>
-      </c>
-      <c r="C24" t="s">
-        <v>110</v>
-      </c>
-      <c r="D24" t="s">
-        <v>82</v>
-      </c>
-      <c r="E24" t="s">
-        <v>73</v>
-      </c>
-      <c r="F24" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>110</v>
-      </c>
-      <c r="B25" t="s">
-        <v>82</v>
-      </c>
-      <c r="C25" t="s">
-        <v>111</v>
-      </c>
-      <c r="D25" t="s">
-        <v>54</v>
-      </c>
-      <c r="E25" t="s">
-        <v>83</v>
-      </c>
-      <c r="F25" t="s">
-        <v>81</v>
-      </c>
-      <c r="G25" t="s">
-        <v>110</v>
-      </c>
       <c r="H25" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
     </row>
   </sheetData>
@@ -2233,557 +2513,557 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:J42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="E41" sqref="E41"/>
+    <sheetView workbookViewId="0" xr3:uid="{51F8DEE0-4D01-5F28-A812-FC0BD7CAC4A5}">
+      <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="21.7109375" customWidth="1"/>
-    <col min="3" max="3" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="24.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="34" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.65625" customWidth="1"/>
+    <col min="3" max="3" width="11.43359375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.1171875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.6796875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.73828125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="24.88671875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="34.03125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>151</v>
+        <v>145</v>
       </c>
       <c r="B1" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="H1" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="I1" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="D1" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="H1" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="I1" s="3" t="s">
-        <v>69</v>
-      </c>
       <c r="J1" s="3" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>152</v>
+        <v>146</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="F2" s="3" t="s">
         <v>6</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
       <c r="H2" s="3"/>
       <c r="I2" s="3"/>
       <c r="J2" s="3"/>
     </row>
-    <row r="3" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>152</v>
+        <v>146</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
       <c r="H3" s="3"/>
       <c r="I3" s="3"/>
       <c r="J3" s="3"/>
     </row>
-    <row r="4" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>152</v>
+        <v>146</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="H4" s="3"/>
       <c r="I4" s="3"/>
       <c r="J4" s="3"/>
     </row>
-    <row r="5" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>152</v>
+        <v>146</v>
       </c>
       <c r="B5" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="G5" s="3" t="s">
         <v>128</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>163</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="F5" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="G5" s="3" t="s">
-        <v>134</v>
       </c>
       <c r="H5" s="3"/>
       <c r="I5" s="3"/>
       <c r="J5" s="3"/>
     </row>
-    <row r="6" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>152</v>
+        <v>146</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>161</v>
+        <v>155</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="F6" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="G6" s="3"/>
       <c r="H6" s="3"/>
       <c r="I6" s="3"/>
       <c r="J6" s="3"/>
     </row>
-    <row r="7" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>152</v>
+        <v>146</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="G7" s="3"/>
       <c r="H7" s="3"/>
       <c r="I7" s="3"/>
       <c r="J7" s="3"/>
     </row>
-    <row r="8" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>152</v>
+        <v>146</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>161</v>
+        <v>155</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="G8" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
       <c r="H8" s="3"/>
       <c r="I8" s="3"/>
       <c r="J8" s="3"/>
     </row>
-    <row r="9" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>152</v>
+        <v>146</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>161</v>
+        <v>155</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="G9" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
       <c r="H9" s="3"/>
       <c r="I9" s="3"/>
       <c r="J9" s="3"/>
     </row>
-    <row r="10" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>152</v>
+        <v>146</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="G10" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
       <c r="H10" s="3"/>
       <c r="I10" s="3"/>
       <c r="J10" s="3"/>
     </row>
-    <row r="11" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>152</v>
+        <v>146</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>139</v>
+        <v>133</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="G11" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
       <c r="H11" s="3"/>
       <c r="I11" s="3"/>
       <c r="J11" s="3"/>
     </row>
-    <row r="12" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>152</v>
+        <v>146</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>140</v>
+        <v>134</v>
       </c>
       <c r="G12" s="3"/>
       <c r="H12" s="3" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
       <c r="I12" s="3" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="J12" s="3"/>
     </row>
-    <row r="13" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>152</v>
+        <v>146</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="D13" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="E13" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="E13" s="3" t="s">
-        <v>78</v>
-      </c>
       <c r="F13" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="G13" s="3"/>
       <c r="H13" s="3"/>
       <c r="I13" s="3"/>
       <c r="J13" s="3"/>
     </row>
-    <row r="14" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>152</v>
+        <v>146</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>139</v>
+        <v>133</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="F14" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="G14" s="3"/>
       <c r="H14" s="3"/>
       <c r="I14" s="3"/>
       <c r="J14" s="3"/>
     </row>
-    <row r="15" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>152</v>
+        <v>146</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="F15" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="G15" s="3"/>
       <c r="H15" s="3"/>
       <c r="I15" s="3"/>
       <c r="J15" s="3"/>
     </row>
-    <row r="16" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>152</v>
+        <v>146</v>
       </c>
       <c r="B16" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="C16" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="C16" s="3" t="s">
-        <v>78</v>
-      </c>
       <c r="D16" s="3" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="F16" s="3" t="s">
-        <v>142</v>
+        <v>136</v>
       </c>
       <c r="G16" s="3" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
       <c r="H16" s="3"/>
       <c r="I16" s="3"/>
       <c r="J16" s="3"/>
     </row>
-    <row r="17" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>152</v>
+        <v>146</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="F17" s="3" t="s">
-        <v>142</v>
+        <v>136</v>
       </c>
       <c r="G17" s="3" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
       <c r="H17" s="3"/>
       <c r="I17" s="3"/>
       <c r="J17" s="3"/>
     </row>
-    <row r="18" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>152</v>
+        <v>146</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="F18" s="3" t="s">
-        <v>142</v>
+        <v>136</v>
       </c>
       <c r="G18" s="3" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
       <c r="H18" s="3"/>
       <c r="I18" s="3"/>
       <c r="J18" s="3"/>
     </row>
-    <row r="19" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>129</v>
+        <v>123</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="F19" s="3" t="s">
         <v>6</v>
       </c>
       <c r="G19" s="3" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
       <c r="H19" s="3"/>
       <c r="I19" s="3"/>
       <c r="J19" s="3"/>
     </row>
-    <row r="20" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>129</v>
+        <v>123</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="F20" s="3" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="G20" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
       <c r="H20" s="3"/>
       <c r="I20" s="3"/>
       <c r="J20" s="3"/>
     </row>
-    <row r="21" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>149</v>
+        <v>143</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="F21" t="s">
         <v>4</v>
@@ -2793,45 +3073,45 @@
       <c r="I21" s="3"/>
       <c r="J21" s="3"/>
     </row>
-    <row r="22" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>149</v>
+        <v>143</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>148</v>
+        <v>142</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="F22" s="3" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
       <c r="G22" s="3"/>
       <c r="H22" s="3"/>
       <c r="I22" s="3"/>
       <c r="J22" s="3"/>
     </row>
-    <row r="23" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>148</v>
+        <v>142</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>150</v>
+        <v>144</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="F23" s="3" t="s">
         <v>4</v>
@@ -2841,21 +3121,21 @@
       <c r="I23" s="3"/>
       <c r="J23" s="3"/>
     </row>
-    <row r="24" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>150</v>
+        <v>144</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="F24" s="3" t="s">
         <v>4</v>
@@ -2865,85 +3145,85 @@
       <c r="I24" s="3"/>
       <c r="J24" s="3"/>
     </row>
-    <row r="25" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>150</v>
+        <v>144</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="D25" s="3" t="s">
         <v>5</v>
       </c>
       <c r="E25" s="3" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="F25" s="3" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
       <c r="G25" s="3"/>
       <c r="H25" s="3"/>
       <c r="I25" s="3"/>
       <c r="J25" s="3"/>
     </row>
-    <row r="26" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>154</v>
+        <v>148</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="E26" s="3" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="F26" s="3" t="s">
         <v>6</v>
       </c>
       <c r="G26" s="3" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="H26" s="3"/>
       <c r="I26" s="3"/>
       <c r="J26" s="3"/>
     </row>
-    <row r="27" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>154</v>
+        <v>148</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="D27" s="3" t="s">
         <v>0</v>
       </c>
       <c r="E27" s="3" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="F27" s="3" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="G27" s="3" t="s">
-        <v>141</v>
+        <v>135</v>
       </c>
       <c r="H27" s="3"/>
       <c r="I27" s="3"/>
       <c r="J27" s="3"/>
     </row>
-    <row r="28" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>154</v>
+        <v>148</v>
       </c>
       <c r="B28" t="s">
         <v>0</v>
@@ -2952,10 +3232,10 @@
         <v>1</v>
       </c>
       <c r="D28" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
       <c r="E28" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="F28" t="s">
         <v>4</v>
@@ -2965,9 +3245,9 @@
       <c r="I28" s="3"/>
       <c r="J28" s="3"/>
     </row>
-    <row r="29" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>154</v>
+        <v>148</v>
       </c>
       <c r="B29" t="s">
         <v>0</v>
@@ -2979,7 +3259,7 @@
         <v>5</v>
       </c>
       <c r="E29" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="F29" t="s">
         <v>4</v>
@@ -2989,275 +3269,275 @@
       <c r="I29" s="3"/>
       <c r="J29" s="3"/>
     </row>
-    <row r="30" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>154</v>
+        <v>148</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>166</v>
+        <v>160</v>
       </c>
       <c r="E30" s="3" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="F30" s="3" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="G30" s="2" t="s">
-        <v>167</v>
+        <v>161</v>
       </c>
       <c r="H30" s="3"/>
       <c r="I30" s="3"/>
       <c r="J30" s="3"/>
     </row>
-    <row r="31" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>154</v>
+        <v>148</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>155</v>
+        <v>149</v>
       </c>
       <c r="E31" s="3" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="F31" s="3" t="s">
-        <v>140</v>
+        <v>134</v>
       </c>
       <c r="G31" s="3"/>
       <c r="H31" s="3" t="s">
-        <v>149</v>
+        <v>143</v>
       </c>
       <c r="I31" s="3" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="J31" s="3"/>
     </row>
-    <row r="32" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>154</v>
+        <v>148</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>129</v>
+        <v>123</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>156</v>
+        <v>150</v>
       </c>
       <c r="E32" s="3" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="F32" s="3" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
       <c r="G32" s="3"/>
       <c r="H32" s="3" t="s">
-        <v>155</v>
+        <v>149</v>
       </c>
       <c r="I32" s="3" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="J32" s="3"/>
     </row>
-    <row r="33" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>154</v>
+        <v>148</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="D33" s="3" t="s">
-        <v>158</v>
+        <v>152</v>
       </c>
       <c r="E33" s="3" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="F33" s="3" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="G33" s="3" t="s">
-        <v>159</v>
+        <v>153</v>
       </c>
       <c r="H33" s="3"/>
       <c r="I33" s="3"/>
       <c r="J33" s="3"/>
     </row>
-    <row r="34" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
+        <v>148</v>
+      </c>
+      <c r="B34" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="C34" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="D34" s="3" t="s">
         <v>154</v>
       </c>
-      <c r="B34" s="3" t="s">
-        <v>156</v>
-      </c>
-      <c r="C34" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="D34" s="3" t="s">
-        <v>160</v>
-      </c>
       <c r="E34" s="3" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="F34" s="3" t="s">
-        <v>140</v>
+        <v>134</v>
       </c>
       <c r="H34" s="3" t="s">
-        <v>158</v>
+        <v>152</v>
       </c>
       <c r="I34" s="3" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="J34" s="3"/>
     </row>
-    <row r="35" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
+        <v>148</v>
+      </c>
+      <c r="B35" s="3" t="s">
         <v>154</v>
       </c>
-      <c r="B35" s="3" t="s">
-        <v>160</v>
-      </c>
       <c r="C35" s="3" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="D35" s="3" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="E35" s="3" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="F35" s="3" t="s">
-        <v>140</v>
+        <v>134</v>
       </c>
       <c r="H35" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
       <c r="I35" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="J35" s="3"/>
     </row>
-    <row r="36" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>154</v>
+        <v>148</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="D36" s="3" t="s">
-        <v>171</v>
+        <v>165</v>
       </c>
       <c r="E36" s="3" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="F36" s="3" t="s">
         <v>6</v>
       </c>
       <c r="G36" s="3" t="s">
-        <v>159</v>
+        <v>153</v>
       </c>
       <c r="H36" s="3"/>
       <c r="I36" s="3"/>
       <c r="J36" s="3"/>
     </row>
-    <row r="37" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>154</v>
+        <v>148</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="D37" s="3" t="s">
-        <v>168</v>
+        <v>162</v>
       </c>
       <c r="E37" s="3" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="F37" s="3" t="s">
-        <v>140</v>
+        <v>134</v>
       </c>
       <c r="H37" s="3" t="s">
-        <v>171</v>
+        <v>165</v>
       </c>
       <c r="I37" s="3" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="J37" s="3"/>
     </row>
-    <row r="38" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>154</v>
+        <v>148</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>166</v>
+        <v>160</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="D38" s="3" t="s">
-        <v>169</v>
+        <v>163</v>
       </c>
       <c r="E38" s="3" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="F38" s="3" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
       <c r="H38" s="3" t="s">
-        <v>168</v>
+        <v>162</v>
       </c>
       <c r="I38" s="3" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="J38" s="3"/>
     </row>
-    <row r="39" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>154</v>
+        <v>148</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="D39" s="3" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
       <c r="E39" s="3" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="F39" s="3" t="s">
-        <v>140</v>
+        <v>134</v>
       </c>
       <c r="H39" s="3" t="s">
-        <v>169</v>
+        <v>163</v>
       </c>
       <c r="I39" s="3" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="40" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B40" s="3"/>
       <c r="C40" s="3"/>
       <c r="D40" s="3"/>
@@ -3267,7 +3547,7 @@
       <c r="I40" s="3"/>
       <c r="J40" s="3"/>
     </row>
-    <row r="42" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B42" s="3"/>
       <c r="C42" s="3"/>
       <c r="D42" s="3"/>
@@ -3284,24 +3564,24 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+    <sheetView tabSelected="1" workbookViewId="0" xr3:uid="{F9CF3CF3-643B-5BE6-8B46-32C596A47465}">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.296875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.43359375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="24.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.6796875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.73828125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="24.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>8</v>
       </c>
@@ -3321,15 +3601,15 @@
         <v>13</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>14</v>
       </c>
       <c r="B2" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="C2" t="s">
         <v>7</v>
@@ -3338,10 +3618,10 @@
         <v>3</v>
       </c>
       <c r="E2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F2" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
     </row>
   </sheetData>
@@ -3350,24 +3630,24 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:G3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView workbookViewId="0" xr3:uid="{78B4E459-6924-5F8B-B7BA-2DD04133E49E}">
       <selection activeCell="D36" sqref="D36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="17" customWidth="1"/>
-    <col min="2" max="2" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="24.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.94921875" customWidth="1"/>
+    <col min="2" max="2" width="11.43359375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.19921875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.6796875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.73828125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="24.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>8</v>
       </c>
@@ -3387,10 +3667,10 @@
         <v>13</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>15</v>
       </c>
@@ -3398,7 +3678,7 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D2" t="s">
         <v>3</v>
@@ -3407,10 +3687,10 @@
         <v>6</v>
       </c>
       <c r="F2" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>15</v>
       </c>
@@ -3424,10 +3704,10 @@
         <v>3</v>
       </c>
       <c r="E3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F3" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
     </row>
   </sheetData>
@@ -3436,204 +3716,360 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G9"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+  <dimension ref="A1:N16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+    <sheetView topLeftCell="C11" workbookViewId="0" xr3:uid="{9B253EF2-77E0-53E3-AE26-4D66ECD923F3}">
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="24.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.296875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.43359375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.6796875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.73828125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="24.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="G1" s="1" t="s">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>145</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="E1" s="3" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>23</v>
-      </c>
-      <c r="B2" t="s">
+      <c r="F1" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="B2" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="H2" s="2"/>
+      <c r="I2" s="2"/>
+      <c r="J2" s="2"/>
+      <c r="K2" s="2"/>
+      <c r="L2" s="2"/>
+      <c r="M2" s="2"/>
+      <c r="N2" s="2"/>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="B3" s="5" t="s">
+        <v>167</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>160</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="G3" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="D2" t="s">
-        <v>44</v>
-      </c>
-      <c r="E2" t="s">
-        <v>17</v>
-      </c>
-      <c r="F2" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>23</v>
-      </c>
-      <c r="B3" t="s">
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="B4" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D4" t="s">
+        <v>37</v>
+      </c>
+      <c r="E4" t="s">
+        <v>1</v>
+      </c>
+      <c r="F4" t="s">
+        <v>6</v>
+      </c>
+      <c r="G4" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="B5" s="4" t="s">
+        <v>160</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>166</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="G5" s="4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="B6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C6" t="s">
+        <v>1</v>
+      </c>
+      <c r="D6" t="s">
+        <v>169</v>
+      </c>
+      <c r="E6" t="s">
+        <v>38</v>
+      </c>
+      <c r="F6" t="s">
+        <v>6</v>
+      </c>
+      <c r="G6" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="B7" t="s">
+        <v>169</v>
+      </c>
+      <c r="C7" t="s">
+        <v>38</v>
+      </c>
+      <c r="D7" t="s">
+        <v>5</v>
+      </c>
+      <c r="E7" t="s">
+        <v>29</v>
+      </c>
+      <c r="F7" t="s">
+        <v>4</v>
+      </c>
+      <c r="G7" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="B8" t="s">
+        <v>169</v>
+      </c>
+      <c r="C8" t="s">
+        <v>38</v>
+      </c>
+      <c r="D8" t="s">
+        <v>22</v>
+      </c>
+      <c r="E8" t="s">
+        <v>1</v>
+      </c>
+      <c r="F8" t="s">
+        <v>4</v>
+      </c>
+      <c r="G8" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="B9" t="s">
+        <v>19</v>
+      </c>
+      <c r="C9" t="s">
+        <v>1</v>
+      </c>
+      <c r="D9" t="s">
+        <v>7</v>
+      </c>
+      <c r="E9" t="s">
+        <v>1</v>
+      </c>
+      <c r="F9" t="s">
+        <v>6</v>
+      </c>
+      <c r="G9" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="B10" t="s">
+        <v>19</v>
+      </c>
+      <c r="C10" t="s">
+        <v>1</v>
+      </c>
+      <c r="D10" t="s">
+        <v>32</v>
+      </c>
+      <c r="E10" t="s">
         <v>3</v>
       </c>
-      <c r="C3" t="s">
-        <v>42</v>
-      </c>
-      <c r="D3" t="s">
+      <c r="F10" t="s">
+        <v>6</v>
+      </c>
+      <c r="G10" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="B11" t="s">
+        <v>21</v>
+      </c>
+      <c r="C11" t="s">
+        <v>3</v>
+      </c>
+      <c r="D11" t="s">
+        <v>175</v>
+      </c>
+      <c r="E11" t="s">
+        <v>38</v>
+      </c>
+      <c r="F11" t="s">
+        <v>6</v>
+      </c>
+      <c r="G11" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="B12" t="s">
+        <v>175</v>
+      </c>
+      <c r="C12" t="s">
+        <v>38</v>
+      </c>
+      <c r="D12" t="s">
+        <v>2</v>
+      </c>
+      <c r="E12" t="s">
         <v>1</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F12" t="s">
         <v>6</v>
       </c>
-      <c r="F3" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="G12" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="B13" t="s">
+        <v>175</v>
+      </c>
+      <c r="C13" t="s">
+        <v>38</v>
+      </c>
+      <c r="D13" t="s">
+        <v>170</v>
+      </c>
+      <c r="E13" t="s">
+        <v>1</v>
+      </c>
+      <c r="F13" t="s">
+        <v>16</v>
+      </c>
+      <c r="G13" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="B14" t="s">
         <v>21</v>
       </c>
-      <c r="B4" t="s">
-        <v>1</v>
-      </c>
-      <c r="C4" t="s">
-        <v>41</v>
-      </c>
-      <c r="D4" t="s">
-        <v>44</v>
-      </c>
-      <c r="E4" t="s">
-        <v>17</v>
-      </c>
-      <c r="F4" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="C14" t="s">
+        <v>3</v>
+      </c>
+      <c r="D14" t="s">
+        <v>172</v>
+      </c>
+      <c r="E14" t="s">
+        <v>38</v>
+      </c>
+      <c r="F14" t="s">
+        <v>77</v>
+      </c>
+      <c r="H14" t="s">
+        <v>169</v>
+      </c>
+      <c r="I14" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="B15" t="s">
         <v>21</v>
       </c>
-      <c r="B5" t="s">
-        <v>1</v>
-      </c>
-      <c r="C5" t="s">
-        <v>31</v>
-      </c>
-      <c r="D5" t="s">
-        <v>44</v>
-      </c>
-      <c r="E5" t="s">
-        <v>6</v>
-      </c>
-      <c r="F5" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>31</v>
-      </c>
-      <c r="B6" t="s">
-        <v>44</v>
-      </c>
-      <c r="C6" t="s">
-        <v>5</v>
-      </c>
-      <c r="D6" t="s">
-        <v>33</v>
-      </c>
-      <c r="E6" t="s">
-        <v>4</v>
-      </c>
-      <c r="F6" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>31</v>
-      </c>
-      <c r="B7" t="s">
-        <v>44</v>
-      </c>
-      <c r="C7" t="s">
-        <v>24</v>
-      </c>
-      <c r="D7" t="s">
-        <v>1</v>
-      </c>
-      <c r="E7" t="s">
-        <v>4</v>
-      </c>
-      <c r="F7" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+      <c r="C15" t="s">
+        <v>3</v>
+      </c>
+      <c r="D15" t="s">
+        <v>173</v>
+      </c>
+      <c r="E15" t="s">
+        <v>3</v>
+      </c>
+      <c r="F15" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="B16" t="s">
         <v>21</v>
       </c>
-      <c r="B8" t="s">
-        <v>1</v>
-      </c>
-      <c r="C8" t="s">
-        <v>7</v>
-      </c>
-      <c r="D8" t="s">
-        <v>1</v>
-      </c>
-      <c r="E8" t="s">
-        <v>6</v>
-      </c>
-      <c r="F8" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>21</v>
-      </c>
-      <c r="B9" t="s">
-        <v>1</v>
-      </c>
-      <c r="C9" t="s">
-        <v>16</v>
-      </c>
-      <c r="D9" t="s">
+      <c r="C16" t="s">
         <v>3</v>
       </c>
-      <c r="E9" t="s">
-        <v>6</v>
-      </c>
-      <c r="F9" t="s">
-        <v>45</v>
+      <c r="D16" t="s">
+        <v>197</v>
+      </c>
+      <c r="E16" t="s">
+        <v>179</v>
+      </c>
+      <c r="F16" t="s">
+        <v>180</v>
+      </c>
+      <c r="G16" t="s">
+        <v>192</v>
       </c>
     </row>
   </sheetData>
@@ -3642,84 +4078,251 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7CE268D0-A74F-044F-AA02-3C2E354D5AA6}">
+  <dimension ref="A1:J11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G1" sqref="G1"/>
+    <sheetView topLeftCell="B7" zoomScaleNormal="150" zoomScaleSheetLayoutView="100" workbookViewId="0" xr3:uid="{826758B4-F8B5-523C-89B5-6D4AD9AB1155}">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="24.85546875" bestFit="1" customWidth="1"/>
-  </cols>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="G1" s="1" t="s">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>145</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="E1" s="3" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>23</v>
-      </c>
+      <c r="F1" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B2" t="s">
-        <v>1</v>
+        <v>177</v>
       </c>
       <c r="C2" t="s">
-        <v>28</v>
+        <v>3</v>
       </c>
       <c r="D2" t="s">
+        <v>178</v>
+      </c>
+      <c r="E2" t="s">
+        <v>179</v>
+      </c>
+      <c r="F2" t="s">
+        <v>180</v>
+      </c>
+      <c r="G2" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B3" t="s">
+        <v>177</v>
+      </c>
+      <c r="C3" t="s">
         <v>3</v>
       </c>
-      <c r="E2" t="s">
-        <v>48</v>
-      </c>
-      <c r="F2" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>28</v>
-      </c>
-      <c r="B3" t="s">
+      <c r="D3" t="s">
+        <v>32</v>
+      </c>
+      <c r="E3" t="s">
+        <v>179</v>
+      </c>
+      <c r="F3" t="s">
+        <v>180</v>
+      </c>
+      <c r="G3" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B4" t="s">
+        <v>177</v>
+      </c>
+      <c r="C4" t="s">
         <v>3</v>
       </c>
-      <c r="C3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D3" t="s">
-        <v>1</v>
-      </c>
-      <c r="E3" t="s">
+      <c r="D4" t="s">
+        <v>183</v>
+      </c>
+      <c r="E4" t="s">
+        <v>179</v>
+      </c>
+      <c r="F4" t="s">
+        <v>180</v>
+      </c>
+      <c r="G4" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B5" t="s">
+        <v>177</v>
+      </c>
+      <c r="C5" t="s">
+        <v>3</v>
+      </c>
+      <c r="D5" t="s">
+        <v>185</v>
+      </c>
+      <c r="E5" t="s">
+        <v>33</v>
+      </c>
+      <c r="F5" t="s">
         <v>6</v>
       </c>
-      <c r="F3" t="s">
-        <v>30</v>
+      <c r="G5" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B6" t="s">
+        <v>187</v>
+      </c>
+      <c r="C6" t="s">
+        <v>179</v>
+      </c>
+      <c r="D6" t="s">
+        <v>188</v>
+      </c>
+      <c r="E6" t="s">
+        <v>189</v>
+      </c>
+      <c r="F6" t="s">
+        <v>190</v>
+      </c>
+      <c r="H6" t="s">
+        <v>185</v>
+      </c>
+      <c r="I6" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B7" t="s">
+        <v>177</v>
+      </c>
+      <c r="C7" t="s">
+        <v>3</v>
+      </c>
+      <c r="D7" t="s">
+        <v>21</v>
+      </c>
+      <c r="E7" t="s">
+        <v>33</v>
+      </c>
+      <c r="F7" t="s">
+        <v>191</v>
+      </c>
+      <c r="H7" t="s">
+        <v>188</v>
+      </c>
+      <c r="I7" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B8" t="s">
+        <v>177</v>
+      </c>
+      <c r="C8" t="s">
+        <v>3</v>
+      </c>
+      <c r="D8" t="s">
+        <v>197</v>
+      </c>
+      <c r="E8" t="s">
+        <v>33</v>
+      </c>
+      <c r="F8" t="s">
+        <v>180</v>
+      </c>
+      <c r="G8" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B9" t="s">
+        <v>177</v>
+      </c>
+      <c r="C9" t="s">
+        <v>3</v>
+      </c>
+      <c r="D9" t="s">
+        <v>193</v>
+      </c>
+      <c r="E9" t="s">
+        <v>189</v>
+      </c>
+      <c r="F9" t="s">
+        <v>6</v>
+      </c>
+      <c r="G9" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B10" t="s">
+        <v>195</v>
+      </c>
+      <c r="C10" t="s">
+        <v>189</v>
+      </c>
+      <c r="D10" t="s">
+        <v>2</v>
+      </c>
+      <c r="E10" t="s">
+        <v>179</v>
+      </c>
+      <c r="F10" t="s">
+        <v>6</v>
+      </c>
+      <c r="G10" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B11" t="s">
+        <v>195</v>
+      </c>
+      <c r="C11" t="s">
+        <v>189</v>
+      </c>
+      <c r="D11" t="s">
+        <v>170</v>
+      </c>
+      <c r="E11" t="s">
+        <v>179</v>
+      </c>
+      <c r="F11" t="s">
+        <v>16</v>
+      </c>
+      <c r="G11" t="s">
+        <v>196</v>
       </c>
     </row>
   </sheetData>
@@ -3728,24 +4331,24 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:G6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+    <sheetView topLeftCell="D3" workbookViewId="0" xr3:uid="{85D5C41F-068E-5C55-9968-509E7C2A5619}">
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.296875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.43359375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="24.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.6796875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.73828125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="24.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>8</v>
       </c>
@@ -3765,107 +4368,107 @@
         <v>13</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D2" t="s">
         <v>3</v>
       </c>
-      <c r="C2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D2" t="s">
-        <v>1</v>
-      </c>
       <c r="E2" t="s">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="F2" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="B3" t="s">
         <v>1</v>
       </c>
       <c r="C3" t="s">
-        <v>56</v>
+        <v>199</v>
       </c>
       <c r="D3" t="s">
-        <v>53</v>
+        <v>3</v>
       </c>
       <c r="E3" t="s">
         <v>6</v>
       </c>
-      <c r="F3" s="2" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F3" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" t="s">
+        <v>1</v>
+      </c>
+      <c r="E4" t="s">
+        <v>6</v>
+      </c>
+      <c r="F4" t="s">
         <v>27</v>
       </c>
-      <c r="B4" t="s">
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>26</v>
+      </c>
+      <c r="B5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5" t="s">
+        <v>32</v>
+      </c>
+      <c r="D5" t="s">
         <v>1</v>
-      </c>
-      <c r="C4" t="s">
-        <v>26</v>
-      </c>
-      <c r="D4" t="s">
-        <v>3</v>
-      </c>
-      <c r="E4" t="s">
-        <v>17</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>56</v>
-      </c>
-      <c r="B5" t="s">
-        <v>53</v>
-      </c>
-      <c r="C5" t="s">
-        <v>24</v>
-      </c>
-      <c r="D5" t="s">
-        <v>54</v>
       </c>
       <c r="E5" t="s">
         <v>6</v>
       </c>
       <c r="F5" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>56</v>
+        <v>26</v>
       </c>
       <c r="B6" t="s">
-        <v>53</v>
+        <v>3</v>
       </c>
       <c r="C6" t="s">
-        <v>57</v>
+        <v>200</v>
       </c>
       <c r="D6" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E6" t="s">
-        <v>17</v>
+        <v>6</v>
       </c>
       <c r="F6" t="s">
-        <v>55</v>
+        <v>201</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Reference steel factory from IEAGHG 2013
</commit_message>
<xml_diff>
--- a/data/steel/SteelUnits_Relationships.xlsx
+++ b/data/steel/SteelUnits_Relationships.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Tanzer/GitHub/BlackBlox/data/steel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4E2D460-3089-F44A-888B-19B87382A8C0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C64AFB6D-7478-A34B-BDC4-FAED4C1ADF47}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-100" yWindow="460" windowWidth="23020" windowHeight="17060" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1200" yWindow="460" windowWidth="23020" windowHeight="17060" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Coke Oven" sheetId="2" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="899" uniqueCount="184">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="878" uniqueCount="179">
   <si>
     <t>CaCO3</t>
   </si>
@@ -193,45 +193,15 @@
     <t>energycontent-LHV</t>
   </si>
   <si>
-    <t>COG from coal energy</t>
-  </si>
-  <si>
-    <t>COG from biofuel energy</t>
-  </si>
-  <si>
-    <t>energy in biofuel (LHV)</t>
-  </si>
-  <si>
-    <t>energy in coking coal (LHV)</t>
-  </si>
-  <si>
-    <t>combustion-lhv-noenergyin</t>
-  </si>
-  <si>
     <t>coking coal__equivelent</t>
   </si>
   <si>
-    <t>COG recovery effeciency</t>
-  </si>
-  <si>
-    <t>energy in coke (LHV)</t>
-  </si>
-  <si>
-    <t>coking coal__lost</t>
-  </si>
-  <si>
-    <t>biofuel__lost</t>
-  </si>
-  <si>
     <t>heat</t>
   </si>
   <si>
     <t>electricity</t>
   </si>
   <si>
-    <t>consumed heat and electricity</t>
-  </si>
-  <si>
     <t>other minerals</t>
   </si>
   <si>
@@ -256,12 +226,6 @@
     <t>biomass cofiring</t>
   </si>
   <si>
-    <t>energy in coke oven gas (LHV)</t>
-  </si>
-  <si>
-    <t>energy inflow total (LHV)</t>
-  </si>
-  <si>
     <t>coke__equiv</t>
   </si>
   <si>
@@ -277,9 +241,6 @@
     <t>energy in coke</t>
   </si>
   <si>
-    <t>Heat Demand (LHV)</t>
-  </si>
-  <si>
     <t>Fe__in sinter</t>
   </si>
   <si>
@@ -367,9 +328,6 @@
     <t>combustion-lhv</t>
   </si>
   <si>
-    <t>BFG recovery efficiency</t>
-  </si>
-  <si>
     <t>blast furnace gas energy</t>
   </si>
   <si>
@@ -578,6 +536,33 @@
   </si>
   <si>
     <t>raw liquid steel</t>
+  </si>
+  <si>
+    <t>CO2__from oxidation`</t>
+  </si>
+  <si>
+    <t>discard</t>
+  </si>
+  <si>
+    <t>not used currently; oxidation assumed to be accounted for in CO2 emissions of combustion</t>
+  </si>
+  <si>
+    <t>BOF heat</t>
+  </si>
+  <si>
+    <t>returnValue</t>
+  </si>
+  <si>
+    <t>CONSUMED heat in steel released as BOF heat</t>
+  </si>
+  <si>
+    <t>energy inflow total</t>
+  </si>
+  <si>
+    <t>energy in coking coal</t>
+  </si>
+  <si>
+    <t>energy in coke oven gas</t>
   </si>
 </sst>
 </file>
@@ -987,10 +972,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:I18"/>
+  <dimension ref="A1:I14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1041,7 +1026,7 @@
         <v>31</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>62</v>
+        <v>70</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>31</v>
@@ -1055,7 +1040,7 @@
     </row>
     <row r="3" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>52</v>
@@ -1075,13 +1060,13 @@
     </row>
     <row r="4" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>52</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>77</v>
+        <v>176</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>52</v>
@@ -1092,13 +1077,13 @@
     </row>
     <row r="5" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
-        <v>77</v>
+        <v>176</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>52</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>57</v>
+        <v>64</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>48</v>
@@ -1115,13 +1100,13 @@
     </row>
     <row r="6" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
-        <v>77</v>
+        <v>176</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>52</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>58</v>
+        <v>177</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>48</v>
@@ -1138,7 +1123,7 @@
     </row>
     <row r="7" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
-        <v>57</v>
+        <v>64</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>48</v>
@@ -1161,7 +1146,7 @@
     </row>
     <row r="8" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
-        <v>58</v>
+        <v>177</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>48</v>
@@ -1184,19 +1169,19 @@
     </row>
     <row r="9" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
-        <v>44</v>
+        <v>176</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>64</v>
+        <v>178</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>52</v>
+        <v>31</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>49</v>
+        <v>6</v>
       </c>
       <c r="F9" s="2" t="s">
         <v>50</v>
@@ -1205,195 +1190,100 @@
       <c r="H9" s="2"/>
       <c r="I9" s="2"/>
     </row>
-    <row r="10" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>48</v>
+        <v>3</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>52</v>
+        <v>1</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>49</v>
+        <v>6</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>50</v>
+        <v>15</v>
       </c>
       <c r="G10" s="2"/>
       <c r="H10" s="2"/>
       <c r="I10" s="2"/>
     </row>
-    <row r="11" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
-        <v>63</v>
+        <v>43</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>52</v>
+        <v>3</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>52</v>
+        <v>1</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>59</v>
+        <v>6</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>61</v>
+        <v>19</v>
       </c>
       <c r="G11" s="2"/>
       <c r="H11" s="2"/>
       <c r="I11" s="2"/>
     </row>
-    <row r="12" spans="1:9" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>56</v>
+        <v>161</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>52</v>
+        <v>31</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="G12" s="2"/>
-      <c r="H12" s="2"/>
+        <v>51</v>
+      </c>
+      <c r="G12" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="H12" s="2" t="s">
+        <v>48</v>
+      </c>
       <c r="I12" s="2"/>
     </row>
-    <row r="13" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="E13" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="F13" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="G13" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="H13" s="2" t="s">
-        <v>52</v>
-      </c>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A13" s="2"/>
+      <c r="B13" s="2"/>
+      <c r="C13" s="2"/>
+      <c r="D13" s="2"/>
+      <c r="E13" s="2"/>
+      <c r="F13" s="2"/>
+      <c r="G13" s="2"/>
+      <c r="H13" s="2"/>
+      <c r="I13" s="2"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A14" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="E14" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="F14" s="2" t="s">
-        <v>15</v>
-      </c>
+      <c r="A14" s="2"/>
+      <c r="B14" s="2"/>
+      <c r="C14" s="2"/>
+      <c r="D14" s="2"/>
+      <c r="E14" s="2"/>
+      <c r="F14" s="2"/>
       <c r="G14" s="2"/>
       <c r="H14" s="2"/>
       <c r="I14" s="2"/>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A15" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="D15" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="E15" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="F15" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="G15" s="2"/>
-      <c r="H15" s="2"/>
-      <c r="I15" s="2"/>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A16" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="D16" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="E16" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="F16" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="G16" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="H16" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="I16" s="2"/>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A17" s="2"/>
-      <c r="B17" s="2"/>
-      <c r="C17" s="2"/>
-      <c r="D17" s="2"/>
-      <c r="E17" s="2"/>
-      <c r="F17" s="2"/>
-      <c r="G17" s="2"/>
-      <c r="H17" s="2"/>
-      <c r="I17" s="2"/>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A18" s="2"/>
-      <c r="B18" s="2"/>
-      <c r="C18" s="2"/>
-      <c r="D18" s="2"/>
-      <c r="E18" s="2"/>
-      <c r="F18" s="2"/>
-      <c r="G18" s="2"/>
-      <c r="H18" s="2"/>
-      <c r="I18" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1422,7 +1312,7 @@
   <sheetData>
     <row r="1" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>121</v>
+        <v>107</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>33</v>
@@ -1454,16 +1344,16 @@
     </row>
     <row r="2" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>123</v>
+        <v>109</v>
       </c>
       <c r="B2" t="s">
-        <v>69</v>
+        <v>59</v>
       </c>
       <c r="C2" t="s">
         <v>3</v>
       </c>
       <c r="D2" t="s">
-        <v>84</v>
+        <v>71</v>
       </c>
       <c r="E2" t="s">
         <v>52</v>
@@ -1472,41 +1362,41 @@
         <v>6</v>
       </c>
       <c r="G2" t="s">
-        <v>70</v>
+        <v>60</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>123</v>
+        <v>109</v>
       </c>
       <c r="B3" t="s">
-        <v>84</v>
+        <v>71</v>
       </c>
       <c r="C3" t="s">
         <v>52</v>
       </c>
       <c r="D3" t="s">
-        <v>95</v>
+        <v>82</v>
       </c>
       <c r="E3" t="s">
         <v>52</v>
       </c>
       <c r="F3" t="s">
-        <v>94</v>
+        <v>81</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>123</v>
+        <v>109</v>
       </c>
       <c r="B4" t="s">
-        <v>87</v>
+        <v>74</v>
       </c>
       <c r="C4" t="s">
         <v>48</v>
       </c>
       <c r="D4" t="s">
-        <v>95</v>
+        <v>82</v>
       </c>
       <c r="E4" t="s">
         <v>52</v>
@@ -1515,75 +1405,75 @@
         <v>6</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>90</v>
+        <v>77</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>123</v>
+        <v>109</v>
       </c>
       <c r="B5" t="s">
-        <v>95</v>
+        <v>82</v>
       </c>
       <c r="C5" t="s">
         <v>52</v>
       </c>
       <c r="D5" t="s">
-        <v>91</v>
+        <v>78</v>
       </c>
       <c r="E5" t="s">
         <v>52</v>
       </c>
       <c r="F5" t="s">
-        <v>86</v>
+        <v>73</v>
       </c>
     </row>
     <row r="6" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>123</v>
+        <v>109</v>
       </c>
       <c r="B6" t="s">
-        <v>91</v>
+        <v>78</v>
       </c>
       <c r="C6" t="s">
         <v>52</v>
       </c>
       <c r="D6" t="s">
-        <v>93</v>
+        <v>80</v>
       </c>
       <c r="E6" t="s">
         <v>52</v>
       </c>
       <c r="F6" t="s">
-        <v>94</v>
+        <v>81</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>123</v>
+        <v>109</v>
       </c>
       <c r="B7" t="s">
-        <v>93</v>
+        <v>80</v>
       </c>
       <c r="C7" t="s">
         <v>52</v>
       </c>
       <c r="D7" t="s">
-        <v>120</v>
+        <v>106</v>
       </c>
       <c r="E7" t="s">
         <v>52</v>
       </c>
       <c r="F7" t="s">
-        <v>86</v>
+        <v>73</v>
       </c>
     </row>
     <row r="8" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>123</v>
+        <v>109</v>
       </c>
       <c r="B8" t="s">
-        <v>120</v>
+        <v>106</v>
       </c>
       <c r="C8" t="s">
         <v>52</v>
@@ -1595,38 +1485,38 @@
         <v>17</v>
       </c>
       <c r="F8" t="s">
-        <v>94</v>
+        <v>81</v>
       </c>
     </row>
     <row r="9" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>123</v>
+        <v>109</v>
       </c>
       <c r="B9" t="s">
-        <v>120</v>
+        <v>106</v>
       </c>
       <c r="C9" t="s">
         <v>52</v>
       </c>
       <c r="D9" t="s">
-        <v>88</v>
+        <v>75</v>
       </c>
       <c r="E9" t="s">
         <v>48</v>
       </c>
       <c r="F9" t="s">
-        <v>86</v>
+        <v>73</v>
       </c>
       <c r="J9" t="s">
-        <v>115</v>
+        <v>101</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>124</v>
+        <v>110</v>
       </c>
       <c r="B10" t="s">
-        <v>69</v>
+        <v>59</v>
       </c>
       <c r="C10" t="s">
         <v>3</v>
@@ -1646,16 +1536,16 @@
     </row>
     <row r="11" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>124</v>
+        <v>110</v>
       </c>
       <c r="B11" t="s">
-        <v>95</v>
+        <v>82</v>
       </c>
       <c r="C11" t="s">
         <v>52</v>
       </c>
       <c r="D11" t="s">
-        <v>85</v>
+        <v>72</v>
       </c>
       <c r="E11" t="s">
         <v>52</v>
@@ -1664,7 +1554,7 @@
         <v>53</v>
       </c>
       <c r="H11" t="s">
-        <v>91</v>
+        <v>78</v>
       </c>
       <c r="I11" t="s">
         <v>52</v>
@@ -1672,25 +1562,25 @@
     </row>
     <row r="12" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>124</v>
+        <v>110</v>
       </c>
       <c r="B12" t="s">
-        <v>87</v>
+        <v>74</v>
       </c>
       <c r="C12" t="s">
         <v>48</v>
       </c>
       <c r="D12" t="s">
-        <v>96</v>
+        <v>83</v>
       </c>
       <c r="E12" t="s">
         <v>52</v>
       </c>
       <c r="F12" t="s">
-        <v>89</v>
+        <v>76</v>
       </c>
       <c r="H12" t="s">
-        <v>85</v>
+        <v>72</v>
       </c>
       <c r="I12" t="s">
         <v>52</v>
@@ -1698,16 +1588,16 @@
     </row>
     <row r="13" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>124</v>
+        <v>110</v>
       </c>
       <c r="B13" t="s">
-        <v>69</v>
+        <v>59</v>
       </c>
       <c r="C13" t="s">
         <v>3</v>
       </c>
       <c r="D13" t="s">
-        <v>97</v>
+        <v>84</v>
       </c>
       <c r="E13" t="s">
         <v>52</v>
@@ -1716,31 +1606,31 @@
         <v>6</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>71</v>
+        <v>61</v>
       </c>
     </row>
     <row r="14" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>124</v>
+        <v>110</v>
       </c>
       <c r="B14" t="s">
-        <v>97</v>
+        <v>84</v>
       </c>
       <c r="C14" t="s">
         <v>52</v>
       </c>
       <c r="D14" t="s">
-        <v>68</v>
+        <v>58</v>
       </c>
       <c r="E14" t="s">
         <v>48</v>
       </c>
       <c r="F14" t="s">
-        <v>89</v>
+        <v>76</v>
       </c>
       <c r="G14" s="2"/>
       <c r="H14" s="2" t="s">
-        <v>96</v>
+        <v>83</v>
       </c>
       <c r="I14" s="2" t="s">
         <v>52</v>
@@ -1748,16 +1638,16 @@
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>122</v>
+        <v>108</v>
       </c>
       <c r="B15" t="s">
-        <v>69</v>
+        <v>59</v>
       </c>
       <c r="C15" t="s">
         <v>3</v>
       </c>
       <c r="D15" t="s">
-        <v>66</v>
+        <v>57</v>
       </c>
       <c r="E15" t="s">
         <v>1</v>
@@ -1771,16 +1661,16 @@
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>122</v>
+        <v>108</v>
       </c>
       <c r="B16" t="s">
-        <v>69</v>
+        <v>59</v>
       </c>
       <c r="C16" t="s">
         <v>31</v>
       </c>
       <c r="D16" t="s">
-        <v>65</v>
+        <v>56</v>
       </c>
       <c r="E16" t="s">
         <v>1</v>
@@ -1789,21 +1679,21 @@
         <v>6</v>
       </c>
       <c r="G16" t="s">
-        <v>83</v>
+        <v>19</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>122</v>
+        <v>108</v>
       </c>
       <c r="B17" t="s">
-        <v>69</v>
+        <v>59</v>
       </c>
       <c r="C17" t="s">
         <v>31</v>
       </c>
       <c r="D17" t="s">
-        <v>78</v>
+        <v>66</v>
       </c>
       <c r="E17" t="s">
         <v>52</v>
@@ -1812,27 +1702,27 @@
         <v>6</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>92</v>
+        <v>79</v>
       </c>
     </row>
     <row r="18" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>122</v>
+        <v>108</v>
       </c>
       <c r="B18" t="s">
-        <v>78</v>
+        <v>66</v>
       </c>
       <c r="C18" t="s">
         <v>52</v>
       </c>
       <c r="D18" t="s">
-        <v>72</v>
+        <v>62</v>
       </c>
       <c r="E18" t="s">
         <v>52</v>
       </c>
       <c r="F18" t="s">
-        <v>73</v>
+        <v>63</v>
       </c>
       <c r="G18" t="s">
         <v>51</v>
@@ -1840,16 +1730,16 @@
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>122</v>
+        <v>108</v>
       </c>
       <c r="B19" t="s">
-        <v>72</v>
+        <v>62</v>
       </c>
       <c r="C19" t="s">
         <v>52</v>
       </c>
       <c r="D19" t="s">
-        <v>74</v>
+        <v>64</v>
       </c>
       <c r="E19" t="s">
         <v>48</v>
@@ -1858,21 +1748,21 @@
         <v>6</v>
       </c>
       <c r="G19" s="2" t="s">
-        <v>75</v>
+        <v>65</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>122</v>
+        <v>108</v>
       </c>
       <c r="B20" t="s">
-        <v>72</v>
+        <v>62</v>
       </c>
       <c r="C20" t="s">
         <v>52</v>
       </c>
       <c r="D20" t="s">
-        <v>82</v>
+        <v>70</v>
       </c>
       <c r="E20" t="s">
         <v>48</v>
@@ -1881,15 +1771,15 @@
         <v>14</v>
       </c>
       <c r="G20" s="2" t="s">
-        <v>75</v>
+        <v>65</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>122</v>
+        <v>108</v>
       </c>
       <c r="B21" t="s">
-        <v>74</v>
+        <v>64</v>
       </c>
       <c r="C21" t="s">
         <v>48</v>
@@ -1901,7 +1791,7 @@
         <v>48</v>
       </c>
       <c r="F21" t="s">
-        <v>73</v>
+        <v>63</v>
       </c>
       <c r="G21" t="s">
         <v>51</v>
@@ -1909,10 +1799,10 @@
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>122</v>
+        <v>108</v>
       </c>
       <c r="B22" t="s">
-        <v>82</v>
+        <v>70</v>
       </c>
       <c r="C22" t="s">
         <v>48</v>
@@ -1924,7 +1814,7 @@
         <v>48</v>
       </c>
       <c r="F22" t="s">
-        <v>73</v>
+        <v>63</v>
       </c>
       <c r="G22" t="s">
         <v>51</v>
@@ -1932,7 +1822,7 @@
     </row>
     <row r="23" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>122</v>
+        <v>108</v>
       </c>
       <c r="B23" t="s">
         <v>44</v>
@@ -1941,13 +1831,13 @@
         <v>48</v>
       </c>
       <c r="D23" t="s">
-        <v>79</v>
+        <v>67</v>
       </c>
       <c r="E23" t="s">
         <v>52</v>
       </c>
       <c r="F23" s="3" t="s">
-        <v>112</v>
+        <v>99</v>
       </c>
       <c r="G23" t="s">
         <v>51</v>
@@ -1955,7 +1845,7 @@
     </row>
     <row r="24" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>122</v>
+        <v>108</v>
       </c>
       <c r="B24" t="s">
         <v>43</v>
@@ -1964,13 +1854,13 @@
         <v>48</v>
       </c>
       <c r="D24" t="s">
-        <v>80</v>
+        <v>68</v>
       </c>
       <c r="E24" t="s">
         <v>52</v>
       </c>
       <c r="F24" s="3" t="s">
-        <v>112</v>
+        <v>99</v>
       </c>
       <c r="G24" t="s">
         <v>51</v>
@@ -1978,16 +1868,16 @@
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>122</v>
+        <v>108</v>
       </c>
       <c r="B25" t="s">
-        <v>80</v>
+        <v>68</v>
       </c>
       <c r="C25" t="s">
         <v>52</v>
       </c>
       <c r="D25" t="s">
-        <v>81</v>
+        <v>69</v>
       </c>
       <c r="E25" t="s">
         <v>31</v>
@@ -1999,7 +1889,7 @@
         <v>51</v>
       </c>
       <c r="H25" t="s">
-        <v>80</v>
+        <v>68</v>
       </c>
       <c r="I25" t="s">
         <v>52</v>
@@ -2007,16 +1897,16 @@
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>122</v>
+        <v>108</v>
       </c>
       <c r="B26" t="s">
-        <v>65</v>
+        <v>56</v>
       </c>
       <c r="C26" t="s">
         <v>48</v>
       </c>
       <c r="D26" t="s">
-        <v>175</v>
+        <v>161</v>
       </c>
       <c r="E26" t="s">
         <v>31</v>
@@ -2025,7 +1915,7 @@
         <v>53</v>
       </c>
       <c r="H26" t="s">
-        <v>66</v>
+        <v>57</v>
       </c>
       <c r="I26" t="s">
         <v>1</v>
@@ -2041,8 +1931,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:J43"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="A27" sqref="A27:XFD27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2058,7 +1948,7 @@
   <sheetData>
     <row r="1" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>121</v>
+        <v>107</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>33</v>
@@ -2090,16 +1980,16 @@
     </row>
     <row r="2" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>122</v>
+        <v>108</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>98</v>
+        <v>85</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>31</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>66</v>
+        <v>57</v>
       </c>
       <c r="E2" s="3" t="s">
         <v>48</v>
@@ -2108,7 +1998,7 @@
         <v>6</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>101</v>
+        <v>88</v>
       </c>
       <c r="H2" s="3"/>
       <c r="I2" s="3"/>
@@ -2116,16 +2006,16 @@
     </row>
     <row r="3" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>122</v>
+        <v>108</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>98</v>
+        <v>85</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>31</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>65</v>
+        <v>56</v>
       </c>
       <c r="E3" s="3" t="s">
         <v>48</v>
@@ -2134,7 +2024,7 @@
         <v>45</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>102</v>
+        <v>89</v>
       </c>
       <c r="H3" s="3"/>
       <c r="I3" s="3"/>
@@ -2142,16 +2032,16 @@
     </row>
     <row r="4" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>122</v>
+        <v>108</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>98</v>
+        <v>85</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>31</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>78</v>
+        <v>66</v>
       </c>
       <c r="E4" s="3" t="s">
         <v>52</v>
@@ -2160,7 +2050,7 @@
         <v>45</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>103</v>
+        <v>90</v>
       </c>
       <c r="H4" s="3"/>
       <c r="I4" s="3"/>
@@ -2168,16 +2058,16 @@
     </row>
     <row r="5" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>122</v>
+        <v>108</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>98</v>
+        <v>85</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>31</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>133</v>
+        <v>119</v>
       </c>
       <c r="E5" s="3" t="s">
         <v>52</v>
@@ -2186,7 +2076,7 @@
         <v>45</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>104</v>
+        <v>91</v>
       </c>
       <c r="H5" s="3"/>
       <c r="I5" s="3"/>
@@ -2194,22 +2084,22 @@
     </row>
     <row r="6" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>122</v>
+        <v>108</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>78</v>
+        <v>66</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>52</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>131</v>
+        <v>117</v>
       </c>
       <c r="E6" s="3" t="s">
         <v>52</v>
       </c>
       <c r="F6" t="s">
-        <v>73</v>
+        <v>63</v>
       </c>
       <c r="G6" s="3"/>
       <c r="H6" s="3"/>
@@ -2218,22 +2108,22 @@
     </row>
     <row r="7" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>122</v>
+        <v>108</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>133</v>
+        <v>119</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>52</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>132</v>
+        <v>118</v>
       </c>
       <c r="E7" s="3" t="s">
         <v>52</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>73</v>
+        <v>63</v>
       </c>
       <c r="G7" s="3"/>
       <c r="H7" s="3"/>
@@ -2242,16 +2132,16 @@
     </row>
     <row r="8" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>122</v>
+        <v>108</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>131</v>
+        <v>117</v>
       </c>
       <c r="C8" s="3" t="s">
         <v>52</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>107</v>
+        <v>94</v>
       </c>
       <c r="E8" s="3" t="s">
         <v>52</v>
@@ -2260,7 +2150,7 @@
         <v>45</v>
       </c>
       <c r="G8" t="s">
-        <v>105</v>
+        <v>92</v>
       </c>
       <c r="H8" s="3"/>
       <c r="I8" s="3"/>
@@ -2268,10 +2158,10 @@
     </row>
     <row r="9" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>122</v>
+        <v>108</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>131</v>
+        <v>117</v>
       </c>
       <c r="C9" s="3" t="s">
         <v>52</v>
@@ -2286,7 +2176,7 @@
         <v>49</v>
       </c>
       <c r="G9" t="s">
-        <v>105</v>
+        <v>92</v>
       </c>
       <c r="H9" s="3"/>
       <c r="I9" s="3"/>
@@ -2294,16 +2184,16 @@
     </row>
     <row r="10" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>122</v>
+        <v>108</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>132</v>
+        <v>118</v>
       </c>
       <c r="C10" s="3" t="s">
         <v>52</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>108</v>
+        <v>95</v>
       </c>
       <c r="E10" s="3" t="s">
         <v>52</v>
@@ -2312,7 +2202,7 @@
         <v>45</v>
       </c>
       <c r="G10" t="s">
-        <v>106</v>
+        <v>93</v>
       </c>
       <c r="H10" s="3"/>
       <c r="I10" s="3"/>
@@ -2320,16 +2210,16 @@
     </row>
     <row r="11" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>122</v>
+        <v>108</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>132</v>
+        <v>118</v>
       </c>
       <c r="C11" s="3" t="s">
         <v>52</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>109</v>
+        <v>96</v>
       </c>
       <c r="E11" s="3" t="s">
         <v>52</v>
@@ -2338,7 +2228,7 @@
         <v>49</v>
       </c>
       <c r="G11" t="s">
-        <v>106</v>
+        <v>93</v>
       </c>
       <c r="H11" s="3"/>
       <c r="I11" s="3"/>
@@ -2346,10 +2236,10 @@
     </row>
     <row r="12" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>122</v>
+        <v>108</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>107</v>
+        <v>94</v>
       </c>
       <c r="C12" s="3" t="s">
         <v>52</v>
@@ -2361,11 +2251,11 @@
         <v>52</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>110</v>
+        <v>97</v>
       </c>
       <c r="G12" s="3"/>
       <c r="H12" s="3" t="s">
-        <v>108</v>
+        <v>95</v>
       </c>
       <c r="I12" s="3" t="s">
         <v>52</v>
@@ -2374,7 +2264,7 @@
     </row>
     <row r="13" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>122</v>
+        <v>108</v>
       </c>
       <c r="B13" s="3" t="s">
         <v>41</v>
@@ -2389,7 +2279,7 @@
         <v>48</v>
       </c>
       <c r="F13" t="s">
-        <v>73</v>
+        <v>63</v>
       </c>
       <c r="G13" s="3"/>
       <c r="H13" s="3"/>
@@ -2398,22 +2288,22 @@
     </row>
     <row r="14" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>122</v>
+        <v>108</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>109</v>
+        <v>96</v>
       </c>
       <c r="C14" s="3" t="s">
         <v>52</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>134</v>
+        <v>120</v>
       </c>
       <c r="E14" s="3" t="s">
         <v>48</v>
       </c>
       <c r="F14" t="s">
-        <v>73</v>
+        <v>63</v>
       </c>
       <c r="G14" s="3"/>
       <c r="H14" s="3"/>
@@ -2422,7 +2312,7 @@
     </row>
     <row r="15" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>122</v>
+        <v>108</v>
       </c>
       <c r="B15" s="3" t="s">
         <v>42</v>
@@ -2437,7 +2327,7 @@
         <v>48</v>
       </c>
       <c r="F15" t="s">
-        <v>73</v>
+        <v>63</v>
       </c>
       <c r="G15" s="3"/>
       <c r="H15" s="3"/>
@@ -2446,7 +2336,7 @@
     </row>
     <row r="16" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>122</v>
+        <v>108</v>
       </c>
       <c r="B16" s="3" t="s">
         <v>43</v>
@@ -2455,50 +2345,46 @@
         <v>48</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>114</v>
+        <v>100</v>
       </c>
       <c r="E16" s="3" t="s">
         <v>17</v>
       </c>
       <c r="F16" s="3" t="s">
-        <v>112</v>
-      </c>
-      <c r="G16" s="3" t="s">
-        <v>113</v>
-      </c>
+        <v>99</v>
+      </c>
+      <c r="G16" s="3"/>
       <c r="H16" s="3"/>
       <c r="I16" s="3"/>
       <c r="J16" s="3"/>
     </row>
     <row r="17" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>122</v>
+        <v>108</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>134</v>
+        <v>120</v>
       </c>
       <c r="C17" s="3" t="s">
         <v>48</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>114</v>
+        <v>100</v>
       </c>
       <c r="E17" s="3" t="s">
         <v>17</v>
       </c>
       <c r="F17" s="3" t="s">
-        <v>112</v>
-      </c>
-      <c r="G17" s="3" t="s">
-        <v>113</v>
-      </c>
+        <v>99</v>
+      </c>
+      <c r="G17" s="3"/>
       <c r="H17" s="3"/>
       <c r="I17" s="3"/>
       <c r="J17" s="3"/>
     </row>
     <row r="18" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>122</v>
+        <v>108</v>
       </c>
       <c r="B18" s="3" t="s">
         <v>44</v>
@@ -2507,33 +2393,31 @@
         <v>48</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>114</v>
+        <v>100</v>
       </c>
       <c r="E18" s="3" t="s">
         <v>17</v>
       </c>
       <c r="F18" s="3" t="s">
-        <v>112</v>
-      </c>
-      <c r="G18" s="3" t="s">
-        <v>113</v>
-      </c>
+        <v>99</v>
+      </c>
+      <c r="G18" s="3"/>
       <c r="H18" s="3"/>
       <c r="I18" s="3"/>
       <c r="J18" s="3"/>
     </row>
     <row r="19" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>122</v>
+        <v>108</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>65</v>
+        <v>56</v>
       </c>
       <c r="C19" s="5" t="s">
         <v>48</v>
       </c>
       <c r="D19" s="5" t="s">
-        <v>175</v>
+        <v>161</v>
       </c>
       <c r="E19" s="5" t="s">
         <v>31</v>
@@ -2543,7 +2427,7 @@
       </c>
       <c r="G19" s="3"/>
       <c r="H19" s="3" t="s">
-        <v>66</v>
+        <v>57</v>
       </c>
       <c r="I19" s="3" t="s">
         <v>48</v>
@@ -2552,16 +2436,16 @@
     </row>
     <row r="20" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>123</v>
+        <v>109</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>98</v>
+        <v>85</v>
       </c>
       <c r="C20" s="3" t="s">
         <v>31</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>99</v>
+        <v>86</v>
       </c>
       <c r="E20" s="3" t="s">
         <v>48</v>
@@ -2570,7 +2454,7 @@
         <v>6</v>
       </c>
       <c r="G20" s="3" t="s">
-        <v>100</v>
+        <v>87</v>
       </c>
       <c r="H20" s="3"/>
       <c r="I20" s="3"/>
@@ -2578,16 +2462,16 @@
     </row>
     <row r="21" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>123</v>
+        <v>109</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>99</v>
+        <v>86</v>
       </c>
       <c r="C21" s="3" t="s">
         <v>48</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>116</v>
+        <v>102</v>
       </c>
       <c r="E21" s="3" t="s">
         <v>52</v>
@@ -2596,7 +2480,7 @@
         <v>45</v>
       </c>
       <c r="G21" t="s">
-        <v>117</v>
+        <v>103</v>
       </c>
       <c r="H21" s="3"/>
       <c r="I21" s="3"/>
@@ -2604,16 +2488,16 @@
     </row>
     <row r="22" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>123</v>
+        <v>109</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>116</v>
+        <v>102</v>
       </c>
       <c r="C22" s="3" t="s">
         <v>52</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>119</v>
+        <v>105</v>
       </c>
       <c r="E22" s="3" t="s">
         <v>52</v>
@@ -2628,22 +2512,22 @@
     </row>
     <row r="23" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>123</v>
+        <v>109</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>119</v>
+        <v>105</v>
       </c>
       <c r="C23" s="3" t="s">
         <v>52</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>118</v>
+        <v>104</v>
       </c>
       <c r="E23" s="3" t="s">
         <v>52</v>
       </c>
       <c r="F23" s="3" t="s">
-        <v>94</v>
+        <v>81</v>
       </c>
       <c r="G23" s="3"/>
       <c r="H23" s="3"/>
@@ -2652,16 +2536,16 @@
     </row>
     <row r="24" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>123</v>
+        <v>109</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>118</v>
+        <v>104</v>
       </c>
       <c r="C24" s="3" t="s">
         <v>52</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>120</v>
+        <v>106</v>
       </c>
       <c r="E24" s="3" t="s">
         <v>52</v>
@@ -2676,19 +2560,19 @@
     </row>
     <row r="25" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>123</v>
+        <v>109</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>120</v>
+        <v>106</v>
       </c>
       <c r="C25" s="3" t="s">
         <v>52</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>88</v>
-      </c>
-      <c r="E25" s="3" t="s">
-        <v>48</v>
+        <v>75</v>
+      </c>
+      <c r="E25" s="5" t="s">
+        <v>171</v>
       </c>
       <c r="F25" s="3" t="s">
         <v>4</v>
@@ -2696,44 +2580,48 @@
       <c r="G25" s="3"/>
       <c r="H25" s="3"/>
       <c r="I25" s="3"/>
-      <c r="J25" s="3"/>
+      <c r="J25" s="5" t="s">
+        <v>172</v>
+      </c>
     </row>
     <row r="26" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>123</v>
+        <v>109</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>120</v>
+        <v>106</v>
       </c>
       <c r="C26" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="D26" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="E26" s="3" t="s">
-        <v>17</v>
+      <c r="D26" s="5" t="s">
+        <v>170</v>
+      </c>
+      <c r="E26" s="5" t="s">
+        <v>171</v>
       </c>
       <c r="F26" s="3" t="s">
-        <v>94</v>
+        <v>81</v>
       </c>
       <c r="G26" s="3"/>
       <c r="H26" s="3"/>
       <c r="I26" s="3"/>
-      <c r="J26" s="5"/>
+      <c r="J26" s="5" t="s">
+        <v>172</v>
+      </c>
     </row>
     <row r="27" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>163</v>
+        <v>149</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>98</v>
+        <v>85</v>
       </c>
       <c r="C27" s="3" t="s">
         <v>31</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>69</v>
+        <v>59</v>
       </c>
       <c r="E27" s="3" t="s">
         <v>48</v>
@@ -2750,10 +2638,10 @@
     </row>
     <row r="28" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>163</v>
+        <v>149</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>98</v>
+        <v>85</v>
       </c>
       <c r="C28" s="3" t="s">
         <v>31</v>
@@ -2768,7 +2656,7 @@
         <v>45</v>
       </c>
       <c r="G28" s="3" t="s">
-        <v>111</v>
+        <v>98</v>
       </c>
       <c r="H28" s="3"/>
       <c r="I28" s="3"/>
@@ -2776,7 +2664,7 @@
     </row>
     <row r="29" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>163</v>
+        <v>149</v>
       </c>
       <c r="B29" t="s">
         <v>0</v>
@@ -2785,7 +2673,7 @@
         <v>1</v>
       </c>
       <c r="D29" t="s">
-        <v>127</v>
+        <v>113</v>
       </c>
       <c r="E29" t="s">
         <v>52</v>
@@ -2800,7 +2688,7 @@
     </row>
     <row r="30" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>163</v>
+        <v>149</v>
       </c>
       <c r="B30" t="s">
         <v>0</v>
@@ -2824,16 +2712,16 @@
     </row>
     <row r="31" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>163</v>
+        <v>149</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>98</v>
+        <v>85</v>
       </c>
       <c r="C31" s="3" t="s">
         <v>31</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>136</v>
+        <v>122</v>
       </c>
       <c r="E31" s="3" t="s">
         <v>52</v>
@@ -2842,7 +2730,7 @@
         <v>45</v>
       </c>
       <c r="G31" s="2" t="s">
-        <v>137</v>
+        <v>123</v>
       </c>
       <c r="H31" s="3"/>
       <c r="I31" s="3"/>
@@ -2850,26 +2738,26 @@
     </row>
     <row r="32" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>163</v>
+        <v>149</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>116</v>
+        <v>102</v>
       </c>
       <c r="C32" s="3" t="s">
         <v>52</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>125</v>
+        <v>111</v>
       </c>
       <c r="E32" s="3" t="s">
         <v>52</v>
       </c>
       <c r="F32" s="3" t="s">
-        <v>110</v>
+        <v>97</v>
       </c>
       <c r="G32" s="3"/>
       <c r="H32" s="3" t="s">
-        <v>119</v>
+        <v>105</v>
       </c>
       <c r="I32" s="3" t="s">
         <v>52</v>
@@ -2878,26 +2766,26 @@
     </row>
     <row r="33" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>163</v>
+        <v>149</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>99</v>
+        <v>86</v>
       </c>
       <c r="C33" s="3" t="s">
         <v>48</v>
       </c>
       <c r="D33" s="3" t="s">
-        <v>126</v>
+        <v>112</v>
       </c>
       <c r="E33" s="3" t="s">
         <v>52</v>
       </c>
       <c r="F33" s="3" t="s">
-        <v>89</v>
+        <v>76</v>
       </c>
       <c r="G33" s="3"/>
       <c r="H33" s="3" t="s">
-        <v>125</v>
+        <v>111</v>
       </c>
       <c r="I33" s="3" t="s">
         <v>52</v>
@@ -2906,16 +2794,16 @@
     </row>
     <row r="34" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>163</v>
+        <v>149</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>69</v>
+        <v>59</v>
       </c>
       <c r="C34" s="3" t="s">
         <v>48</v>
       </c>
       <c r="D34" s="3" t="s">
-        <v>128</v>
+        <v>114</v>
       </c>
       <c r="E34" s="3" t="s">
         <v>52</v>
@@ -2924,7 +2812,7 @@
         <v>49</v>
       </c>
       <c r="G34" s="3" t="s">
-        <v>129</v>
+        <v>115</v>
       </c>
       <c r="H34" s="3"/>
       <c r="I34" s="3"/>
@@ -2932,25 +2820,25 @@
     </row>
     <row r="35" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>163</v>
+        <v>149</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>126</v>
+        <v>112</v>
       </c>
       <c r="C35" s="3" t="s">
         <v>52</v>
       </c>
       <c r="D35" s="3" t="s">
-        <v>130</v>
+        <v>116</v>
       </c>
       <c r="E35" s="3" t="s">
         <v>52</v>
       </c>
       <c r="F35" s="3" t="s">
-        <v>110</v>
+        <v>97</v>
       </c>
       <c r="H35" s="3" t="s">
-        <v>128</v>
+        <v>114</v>
       </c>
       <c r="I35" s="3" t="s">
         <v>52</v>
@@ -2959,25 +2847,25 @@
     </row>
     <row r="36" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>163</v>
+        <v>149</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>130</v>
+        <v>116</v>
       </c>
       <c r="C36" s="3" t="s">
         <v>52</v>
       </c>
       <c r="D36" s="3" t="s">
-        <v>140</v>
+        <v>126</v>
       </c>
       <c r="E36" s="3" t="s">
         <v>52</v>
       </c>
       <c r="F36" s="3" t="s">
-        <v>110</v>
+        <v>97</v>
       </c>
       <c r="H36" t="s">
-        <v>127</v>
+        <v>113</v>
       </c>
       <c r="I36" t="s">
         <v>52</v>
@@ -2986,16 +2874,16 @@
     </row>
     <row r="37" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>163</v>
+        <v>149</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>69</v>
+        <v>59</v>
       </c>
       <c r="C37" s="3" t="s">
         <v>48</v>
       </c>
       <c r="D37" s="3" t="s">
-        <v>141</v>
+        <v>127</v>
       </c>
       <c r="E37" s="3" t="s">
         <v>52</v>
@@ -3004,7 +2892,7 @@
         <v>6</v>
       </c>
       <c r="G37" s="3" t="s">
-        <v>129</v>
+        <v>115</v>
       </c>
       <c r="H37" s="3"/>
       <c r="I37" s="3"/>
@@ -3012,25 +2900,25 @@
     </row>
     <row r="38" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>163</v>
+        <v>149</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>116</v>
+        <v>102</v>
       </c>
       <c r="C38" s="3" t="s">
         <v>52</v>
       </c>
       <c r="D38" s="3" t="s">
-        <v>138</v>
+        <v>124</v>
       </c>
       <c r="E38" s="3" t="s">
         <v>52</v>
       </c>
       <c r="F38" s="3" t="s">
-        <v>110</v>
+        <v>97</v>
       </c>
       <c r="H38" s="3" t="s">
-        <v>141</v>
+        <v>127</v>
       </c>
       <c r="I38" s="3" t="s">
         <v>52</v>
@@ -3039,25 +2927,25 @@
     </row>
     <row r="39" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>163</v>
+        <v>149</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>136</v>
+        <v>124</v>
       </c>
       <c r="C39" s="3" t="s">
         <v>52</v>
       </c>
       <c r="D39" s="3" t="s">
-        <v>139</v>
+        <v>125</v>
       </c>
       <c r="E39" s="3" t="s">
         <v>52</v>
       </c>
       <c r="F39" s="3" t="s">
-        <v>89</v>
+        <v>76</v>
       </c>
       <c r="H39" s="3" t="s">
-        <v>138</v>
+        <v>122</v>
       </c>
       <c r="I39" s="3" t="s">
         <v>52</v>
@@ -3066,25 +2954,25 @@
     </row>
     <row r="40" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>163</v>
+        <v>149</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>140</v>
+        <v>126</v>
       </c>
       <c r="C40" s="3" t="s">
         <v>52</v>
       </c>
       <c r="D40" s="3" t="s">
-        <v>135</v>
+        <v>121</v>
       </c>
       <c r="E40" s="3" t="s">
         <v>31</v>
       </c>
       <c r="F40" s="3" t="s">
-        <v>110</v>
+        <v>97</v>
       </c>
       <c r="H40" s="3" t="s">
-        <v>139</v>
+        <v>125</v>
       </c>
       <c r="I40" s="3" t="s">
         <v>52</v>
@@ -3118,10 +3006,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
-  <dimension ref="A1:J18"/>
+  <dimension ref="A1:J19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3137,7 +3025,7 @@
   <sheetData>
     <row r="1" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>121</v>
+        <v>107</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>33</v>
@@ -3169,16 +3057,16 @@
     </row>
     <row r="2" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
-        <v>162</v>
+        <v>148</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>165</v>
+        <v>151</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>24</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>183</v>
+        <v>169</v>
       </c>
       <c r="E2" s="4" t="s">
         <v>3</v>
@@ -3187,21 +3075,21 @@
         <v>14</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>158</v>
+        <v>144</v>
       </c>
     </row>
     <row r="3" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
-        <v>162</v>
+        <v>148</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>165</v>
+        <v>151</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>24</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>98</v>
+        <v>85</v>
       </c>
       <c r="E3" s="4" t="s">
         <v>1</v>
@@ -3215,16 +3103,16 @@
     </row>
     <row r="4" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
-        <v>162</v>
+        <v>148</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>165</v>
+        <v>151</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>24</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>166</v>
+        <v>152</v>
       </c>
       <c r="E4" s="4" t="s">
         <v>1</v>
@@ -3238,16 +3126,16 @@
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
-        <v>123</v>
+        <v>109</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>98</v>
+        <v>85</v>
       </c>
       <c r="C5" t="s">
         <v>1</v>
       </c>
       <c r="D5" t="s">
-        <v>142</v>
+        <v>128</v>
       </c>
       <c r="E5" t="s">
         <v>24</v>
@@ -3261,10 +3149,10 @@
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
-        <v>123</v>
+        <v>109</v>
       </c>
       <c r="B6" t="s">
-        <v>142</v>
+        <v>128</v>
       </c>
       <c r="C6" t="s">
         <v>24</v>
@@ -3284,19 +3172,19 @@
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
-        <v>123</v>
+        <v>109</v>
       </c>
       <c r="B7" t="s">
-        <v>142</v>
+        <v>128</v>
       </c>
       <c r="C7" t="s">
         <v>24</v>
       </c>
       <c r="D7" t="s">
-        <v>171</v>
+        <v>157</v>
       </c>
       <c r="E7" t="s">
-        <v>159</v>
+        <v>145</v>
       </c>
       <c r="F7" t="s">
         <v>4</v>
@@ -3307,65 +3195,65 @@
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
-        <v>123</v>
+        <v>109</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>183</v>
+        <v>169</v>
       </c>
       <c r="C8" t="s">
         <v>3</v>
       </c>
       <c r="D8" t="s">
-        <v>173</v>
+        <v>159</v>
       </c>
       <c r="E8" t="s">
-        <v>146</v>
+        <v>132</v>
       </c>
       <c r="F8" t="s">
-        <v>147</v>
+        <v>133</v>
       </c>
       <c r="G8" t="s">
-        <v>155</v>
+        <v>141</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
-        <v>123</v>
+        <v>109</v>
       </c>
       <c r="B9" t="s">
-        <v>171</v>
+        <v>157</v>
       </c>
       <c r="C9" t="s">
-        <v>159</v>
+        <v>145</v>
       </c>
       <c r="D9" t="s">
-        <v>172</v>
+        <v>158</v>
       </c>
       <c r="E9" t="s">
         <v>20</v>
       </c>
       <c r="F9" t="s">
-        <v>144</v>
+        <v>130</v>
       </c>
       <c r="H9" t="s">
-        <v>173</v>
+        <v>159</v>
       </c>
       <c r="I9" t="s">
-        <v>146</v>
+        <v>132</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
-        <v>122</v>
+        <v>108</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>183</v>
+        <v>169</v>
       </c>
       <c r="C10" t="s">
         <v>31</v>
       </c>
       <c r="D10" t="s">
-        <v>66</v>
+        <v>57</v>
       </c>
       <c r="E10" t="s">
         <v>1</v>
@@ -3379,191 +3267,211 @@
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11" s="4" t="s">
-        <v>122</v>
+        <v>108</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>183</v>
+        <v>169</v>
       </c>
       <c r="C11" t="s">
         <v>31</v>
       </c>
       <c r="D11" t="s">
-        <v>65</v>
+        <v>173</v>
       </c>
       <c r="E11" t="s">
-        <v>3</v>
+        <v>31</v>
       </c>
       <c r="F11" t="s">
         <v>6</v>
       </c>
       <c r="G11" t="s">
-        <v>161</v>
+        <v>147</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A12" s="4" t="s">
-        <v>122</v>
-      </c>
-      <c r="B12" s="4" t="s">
-        <v>66</v>
+        <v>108</v>
+      </c>
+      <c r="B12" t="s">
+        <v>173</v>
       </c>
       <c r="C12" t="s">
+        <v>3</v>
+      </c>
+      <c r="D12" t="s">
+        <v>175</v>
+      </c>
+      <c r="E12" t="s">
         <v>48</v>
       </c>
-      <c r="D12" t="s">
+      <c r="F12" t="s">
         <v>174</v>
-      </c>
-      <c r="E12" t="s">
-        <v>31</v>
-      </c>
-      <c r="F12" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A13" s="4" t="s">
-        <v>124</v>
+        <v>108</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>183</v>
+        <v>57</v>
       </c>
       <c r="C13" t="s">
-        <v>3</v>
+        <v>48</v>
       </c>
       <c r="D13" t="s">
-        <v>167</v>
+        <v>160</v>
       </c>
       <c r="E13" t="s">
-        <v>24</v>
+        <v>31</v>
       </c>
       <c r="F13" t="s">
-        <v>6</v>
-      </c>
-      <c r="G13" t="s">
-        <v>143</v>
+        <v>26</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A14" s="4" t="s">
-        <v>124</v>
-      </c>
-      <c r="B14" t="s">
-        <v>167</v>
+        <v>110</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>169</v>
       </c>
       <c r="C14" t="s">
+        <v>3</v>
+      </c>
+      <c r="D14" t="s">
+        <v>153</v>
+      </c>
+      <c r="E14" t="s">
         <v>24</v>
-      </c>
-      <c r="D14" t="s">
-        <v>2</v>
-      </c>
-      <c r="E14" t="s">
-        <v>1</v>
       </c>
       <c r="F14" t="s">
         <v>6</v>
       </c>
       <c r="G14" t="s">
-        <v>145</v>
+        <v>129</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A15" s="4" t="s">
-        <v>124</v>
+        <v>110</v>
       </c>
       <c r="B15" t="s">
-        <v>167</v>
+        <v>153</v>
       </c>
       <c r="C15" t="s">
         <v>24</v>
       </c>
       <c r="D15" t="s">
-        <v>168</v>
+        <v>2</v>
       </c>
       <c r="E15" t="s">
         <v>1</v>
       </c>
       <c r="F15" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="G15" t="s">
-        <v>145</v>
+        <v>131</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A16" s="4" t="s">
-        <v>163</v>
-      </c>
-      <c r="B16" s="4" t="s">
-        <v>183</v>
+        <v>110</v>
+      </c>
+      <c r="B16" t="s">
+        <v>153</v>
       </c>
       <c r="C16" t="s">
-        <v>3</v>
+        <v>24</v>
       </c>
       <c r="D16" t="s">
-        <v>170</v>
+        <v>154</v>
       </c>
       <c r="E16" t="s">
-        <v>24</v>
+        <v>1</v>
       </c>
       <c r="F16" t="s">
-        <v>53</v>
-      </c>
-      <c r="H16" t="s">
-        <v>142</v>
-      </c>
-      <c r="I16" t="s">
-        <v>24</v>
+        <v>14</v>
+      </c>
+      <c r="G16" t="s">
+        <v>131</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A17" s="4" t="s">
-        <v>163</v>
+        <v>149</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>165</v>
+        <v>169</v>
       </c>
       <c r="C17" t="s">
-        <v>24</v>
+        <v>3</v>
       </c>
       <c r="D17" t="s">
-        <v>169</v>
+        <v>156</v>
       </c>
       <c r="E17" t="s">
         <v>24</v>
       </c>
       <c r="F17" t="s">
-        <v>144</v>
+        <v>53</v>
       </c>
       <c r="H17" t="s">
-        <v>170</v>
-      </c>
-      <c r="I17" s="4" t="s">
+        <v>128</v>
+      </c>
+      <c r="I17" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18" s="4" t="s">
-        <v>163</v>
-      </c>
-      <c r="B18" t="s">
-        <v>169</v>
+        <v>149</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>151</v>
       </c>
       <c r="C18" t="s">
-        <v>159</v>
+        <v>24</v>
       </c>
       <c r="D18" t="s">
-        <v>163</v>
+        <v>155</v>
       </c>
       <c r="E18" t="s">
+        <v>24</v>
+      </c>
+      <c r="F18" t="s">
+        <v>130</v>
+      </c>
+      <c r="H18" t="s">
+        <v>156</v>
+      </c>
+      <c r="I18" s="4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A19" s="4" t="s">
+        <v>149</v>
+      </c>
+      <c r="B19" t="s">
+        <v>155</v>
+      </c>
+      <c r="C19" t="s">
+        <v>145</v>
+      </c>
+      <c r="D19" t="s">
+        <v>149</v>
+      </c>
+      <c r="E19" t="s">
         <v>3</v>
       </c>
-      <c r="F18" t="s">
+      <c r="F19" t="s">
         <v>53</v>
       </c>
-      <c r="H18" t="s">
-        <v>167</v>
-      </c>
-      <c r="I18" t="s">
+      <c r="H19" t="s">
+        <v>153</v>
+      </c>
+      <c r="I19" t="s">
         <v>24</v>
       </c>
     </row>
@@ -3577,7 +3485,7 @@
   <dimension ref="A1:J15"/>
   <sheetViews>
     <sheetView zoomScale="135" zoomScaleNormal="140" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+      <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3589,7 +3497,7 @@
   <sheetData>
     <row r="1" spans="1:10" s="5" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="5" t="s">
-        <v>121</v>
+        <v>107</v>
       </c>
       <c r="B1" s="5" t="s">
         <v>33</v>
@@ -3621,88 +3529,88 @@
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>122</v>
+        <v>108</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>164</v>
+        <v>150</v>
       </c>
       <c r="C2" t="s">
         <v>3</v>
       </c>
       <c r="D2" t="s">
-        <v>66</v>
+        <v>57</v>
       </c>
       <c r="E2" t="s">
-        <v>146</v>
+        <v>132</v>
       </c>
       <c r="F2" t="s">
-        <v>147</v>
+        <v>133</v>
       </c>
       <c r="G2" t="s">
-        <v>148</v>
+        <v>134</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>122</v>
+        <v>108</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>164</v>
+        <v>150</v>
       </c>
       <c r="C3" t="s">
         <v>3</v>
       </c>
       <c r="D3" t="s">
-        <v>65</v>
+        <v>56</v>
       </c>
       <c r="E3" t="s">
-        <v>146</v>
+        <v>132</v>
       </c>
       <c r="F3" t="s">
-        <v>147</v>
+        <v>133</v>
       </c>
       <c r="G3" t="s">
-        <v>149</v>
+        <v>135</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>122</v>
+        <v>108</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>66</v>
+        <v>57</v>
       </c>
       <c r="C4" t="s">
         <v>48</v>
       </c>
       <c r="D4" t="s">
-        <v>175</v>
+        <v>161</v>
       </c>
       <c r="E4" t="s">
         <v>31</v>
       </c>
       <c r="F4" t="s">
-        <v>153</v>
+        <v>139</v>
       </c>
       <c r="H4" t="s">
-        <v>65</v>
+        <v>56</v>
       </c>
       <c r="I4" t="s">
-        <v>146</v>
+        <v>132</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>162</v>
+        <v>148</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>164</v>
+        <v>150</v>
       </c>
       <c r="C5" t="s">
         <v>3</v>
       </c>
       <c r="D5" t="s">
-        <v>166</v>
+        <v>152</v>
       </c>
       <c r="E5" t="s">
         <v>3</v>
@@ -3711,30 +3619,30 @@
         <v>6</v>
       </c>
       <c r="G5" t="s">
-        <v>160</v>
+        <v>146</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>162</v>
+        <v>148</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>164</v>
+        <v>150</v>
       </c>
       <c r="C6" t="s">
         <v>31</v>
       </c>
       <c r="D6" t="s">
-        <v>176</v>
+        <v>162</v>
       </c>
       <c r="E6" t="s">
+        <v>138</v>
+      </c>
+      <c r="F6" t="s">
+        <v>139</v>
+      </c>
+      <c r="H6" t="s">
         <v>152</v>
-      </c>
-      <c r="F6" t="s">
-        <v>153</v>
-      </c>
-      <c r="H6" t="s">
-        <v>166</v>
       </c>
       <c r="I6" t="s">
         <v>3</v>
@@ -3742,39 +3650,39 @@
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
+        <v>148</v>
+      </c>
+      <c r="B7" t="s">
         <v>162</v>
       </c>
-      <c r="B7" t="s">
-        <v>176</v>
-      </c>
       <c r="C7" t="s">
-        <v>152</v>
+        <v>138</v>
       </c>
       <c r="D7" t="s">
-        <v>179</v>
+        <v>165</v>
       </c>
       <c r="E7" t="s">
-        <v>146</v>
+        <v>132</v>
       </c>
       <c r="F7" t="s">
-        <v>147</v>
+        <v>133</v>
       </c>
       <c r="G7" t="s">
-        <v>150</v>
+        <v>136</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
+        <v>148</v>
+      </c>
+      <c r="B8" t="s">
         <v>162</v>
       </c>
-      <c r="B8" t="s">
-        <v>176</v>
-      </c>
       <c r="C8" t="s">
-        <v>152</v>
+        <v>138</v>
       </c>
       <c r="D8" t="s">
-        <v>177</v>
+        <v>163</v>
       </c>
       <c r="E8" t="s">
         <v>20</v>
@@ -3783,30 +3691,30 @@
         <v>6</v>
       </c>
       <c r="G8" t="s">
-        <v>151</v>
+        <v>137</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>162</v>
+        <v>148</v>
       </c>
       <c r="B9" t="s">
-        <v>179</v>
+        <v>165</v>
       </c>
       <c r="C9" t="s">
-        <v>146</v>
+        <v>132</v>
       </c>
       <c r="D9" t="s">
-        <v>178</v>
+        <v>164</v>
       </c>
       <c r="E9" t="s">
-        <v>152</v>
+        <v>138</v>
       </c>
       <c r="F9" t="s">
-        <v>153</v>
+        <v>139</v>
       </c>
       <c r="H9" t="s">
-        <v>177</v>
+        <v>163</v>
       </c>
       <c r="I9" t="s">
         <v>20</v>
@@ -3814,149 +3722,149 @@
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
+        <v>148</v>
+      </c>
+      <c r="B10" t="s">
         <v>162</v>
       </c>
-      <c r="B10" t="s">
-        <v>176</v>
-      </c>
       <c r="C10" t="s">
-        <v>152</v>
+        <v>138</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>183</v>
+        <v>169</v>
       </c>
       <c r="E10" t="s">
         <v>20</v>
       </c>
       <c r="F10" t="s">
-        <v>154</v>
+        <v>140</v>
       </c>
       <c r="H10" t="s">
-        <v>178</v>
+        <v>164</v>
       </c>
       <c r="I10" t="s">
-        <v>152</v>
+        <v>138</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>124</v>
+        <v>110</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>164</v>
+        <v>150</v>
       </c>
       <c r="C11" t="s">
         <v>3</v>
       </c>
       <c r="D11" t="s">
-        <v>167</v>
+        <v>153</v>
       </c>
       <c r="E11" t="s">
-        <v>152</v>
+        <v>138</v>
       </c>
       <c r="F11" t="s">
         <v>6</v>
       </c>
       <c r="G11" t="s">
-        <v>156</v>
+        <v>142</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>124</v>
+        <v>110</v>
       </c>
       <c r="B12" t="s">
-        <v>167</v>
+        <v>153</v>
       </c>
       <c r="C12" t="s">
-        <v>152</v>
+        <v>138</v>
       </c>
       <c r="D12" t="s">
         <v>2</v>
       </c>
       <c r="E12" t="s">
-        <v>146</v>
+        <v>132</v>
       </c>
       <c r="F12" t="s">
         <v>6</v>
       </c>
       <c r="G12" t="s">
-        <v>145</v>
+        <v>131</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>124</v>
+        <v>110</v>
       </c>
       <c r="B13" t="s">
-        <v>167</v>
+        <v>153</v>
       </c>
       <c r="C13" t="s">
-        <v>152</v>
+        <v>138</v>
       </c>
       <c r="D13" t="s">
-        <v>168</v>
+        <v>154</v>
       </c>
       <c r="E13" t="s">
-        <v>146</v>
+        <v>132</v>
       </c>
       <c r="F13" t="s">
         <v>14</v>
       </c>
       <c r="G13" t="s">
-        <v>145</v>
+        <v>131</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>163</v>
+        <v>149</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>164</v>
+        <v>150</v>
       </c>
       <c r="C14" t="s">
         <v>3</v>
       </c>
       <c r="D14" t="s">
-        <v>173</v>
+        <v>159</v>
       </c>
       <c r="E14" t="s">
         <v>20</v>
       </c>
       <c r="F14" t="s">
-        <v>147</v>
+        <v>133</v>
       </c>
       <c r="G14" t="s">
-        <v>155</v>
+        <v>141</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>163</v>
+        <v>149</v>
       </c>
       <c r="B15" t="s">
-        <v>167</v>
+        <v>153</v>
       </c>
       <c r="C15" t="s">
         <v>52</v>
       </c>
       <c r="D15" t="s">
-        <v>163</v>
+        <v>149</v>
       </c>
       <c r="E15" t="s">
         <v>31</v>
       </c>
       <c r="F15" t="s">
-        <v>153</v>
+        <v>139</v>
       </c>
       <c r="H15" t="s">
-        <v>173</v>
+        <v>159</v>
       </c>
       <c r="I15" t="s">
         <v>20</v>
       </c>
       <c r="J15" t="s">
-        <v>180</v>
+        <v>166</v>
       </c>
     </row>
   </sheetData>
@@ -3984,7 +3892,7 @@
   <sheetData>
     <row r="1" spans="1:10" s="5" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="5" t="s">
-        <v>121</v>
+        <v>107</v>
       </c>
       <c r="B1" s="5" t="s">
         <v>33</v>
@@ -4016,16 +3924,16 @@
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>162</v>
+        <v>148</v>
       </c>
       <c r="B2" t="s">
-        <v>164</v>
+        <v>150</v>
       </c>
       <c r="C2" t="s">
         <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>181</v>
+        <v>167</v>
       </c>
       <c r="E2" t="s">
         <v>3</v>
@@ -4034,21 +3942,21 @@
         <v>14</v>
       </c>
       <c r="G2" t="s">
-        <v>160</v>
+        <v>146</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>162</v>
+        <v>148</v>
       </c>
       <c r="B3" t="s">
-        <v>164</v>
+        <v>150</v>
       </c>
       <c r="C3" t="s">
         <v>1</v>
       </c>
       <c r="D3" t="s">
-        <v>166</v>
+        <v>152</v>
       </c>
       <c r="E3" t="s">
         <v>52</v>
@@ -4057,21 +3965,21 @@
         <v>6</v>
       </c>
       <c r="G3" t="s">
-        <v>160</v>
+        <v>146</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>162</v>
+        <v>148</v>
       </c>
       <c r="B4" t="s">
-        <v>181</v>
+        <v>167</v>
       </c>
       <c r="C4" t="s">
         <v>3</v>
       </c>
       <c r="D4" t="s">
-        <v>173</v>
+        <v>159</v>
       </c>
       <c r="E4" t="s">
         <v>1</v>
@@ -4080,21 +3988,21 @@
         <v>6</v>
       </c>
       <c r="G4" t="s">
-        <v>157</v>
+        <v>143</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>162</v>
+        <v>148</v>
       </c>
       <c r="B5" t="s">
-        <v>166</v>
+        <v>152</v>
       </c>
       <c r="C5" t="s">
         <v>52</v>
       </c>
       <c r="D5" t="s">
-        <v>182</v>
+        <v>168</v>
       </c>
       <c r="E5" t="s">
         <v>31</v>
@@ -4103,7 +4011,7 @@
         <v>53</v>
       </c>
       <c r="H5" t="s">
-        <v>173</v>
+        <v>159</v>
       </c>
       <c r="I5" t="s">
         <v>1</v>
@@ -4111,16 +4019,16 @@
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>122</v>
+        <v>108</v>
       </c>
       <c r="B6" t="s">
-        <v>181</v>
+        <v>167</v>
       </c>
       <c r="C6" t="s">
         <v>3</v>
       </c>
       <c r="D6" t="s">
-        <v>66</v>
+        <v>57</v>
       </c>
       <c r="E6" t="s">
         <v>1</v>
@@ -4134,16 +4042,16 @@
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>122</v>
+        <v>108</v>
       </c>
       <c r="B7" t="s">
-        <v>181</v>
+        <v>167</v>
       </c>
       <c r="C7" t="s">
         <v>3</v>
       </c>
       <c r="D7" t="s">
-        <v>65</v>
+        <v>56</v>
       </c>
       <c r="E7" t="s">
         <v>1</v>
@@ -4152,21 +4060,21 @@
         <v>6</v>
       </c>
       <c r="G7" t="s">
-        <v>149</v>
+        <v>135</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>122</v>
+        <v>108</v>
       </c>
       <c r="B8" t="s">
-        <v>65</v>
+        <v>56</v>
       </c>
       <c r="C8" t="s">
         <v>48</v>
       </c>
       <c r="D8" t="s">
-        <v>175</v>
+        <v>161</v>
       </c>
       <c r="E8" t="s">
         <v>31</v>
@@ -4175,7 +4083,7 @@
         <v>53</v>
       </c>
       <c r="H8" t="s">
-        <v>66</v>
+        <v>57</v>
       </c>
       <c r="I8" t="s">
         <v>1</v>
@@ -4190,7 +4098,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:G4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>

</xml_diff>